<commit_message>
Update input data and script files regarding molecular biology data treatment
</commit_message>
<xml_diff>
--- a/input_data/Manuscript_4_removal_efficiency.xlsx
+++ b/input_data/Manuscript_4_removal_efficiency.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rita\Documents\R\Manuscript_4\input_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rita\Documents\R\amendment_micropollutant_biodegradation_aquifer\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF6AF8D-B94E-44B5-8D5A-41FAC51BAF94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B9034C2-6D1B-4B1C-AFED-B23648C0BDD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="removal_efficiency" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">removal_efficiency!$A$1:$AF$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">removal_efficiency!$A$1:$U$425</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -472,10 +472,13 @@
   <dimension ref="A1:U425"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S262" sqref="S262"/>
+      <selection activeCell="A425" activeCellId="11" sqref="A271:XFD271 A293:XFD293 A305:XFD305 A317:XFD317 A329:XFD329 A341:XFD341 A355:XFD355 A377:XFD377 A389:XFD389 A401:XFD401 A413:XFD413 A425:XFD425"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -17518,58 +17521,58 @@
         <v>29</v>
       </c>
       <c r="D263" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E263">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F263">
-        <v>50</v>
+        <v>2.5</v>
       </c>
       <c r="G263" s="1">
-        <v>100</v>
+        <v>-8.0357142857142883</v>
       </c>
       <c r="H263" s="1">
-        <v>15.789473684210513</v>
+        <v>10.796915167095104</v>
       </c>
       <c r="I263" s="1">
-        <v>-8.6642599277978203</v>
+        <v>-169.92287917737789</v>
       </c>
       <c r="J263" s="1">
-        <v>-1.1756715966961206</v>
+        <v>1.2089007620510992</v>
       </c>
       <c r="K263" s="1">
-        <v>5.4545454545454515</v>
+        <v>4.3859649122807012</v>
       </c>
       <c r="L263" s="1">
-        <v>2.2257326566507274</v>
+        <v>4.5796989571422255</v>
       </c>
       <c r="M263" s="1">
-        <v>-0.38303354394105016</v>
+        <v>0.72894054446455525</v>
       </c>
       <c r="N263" s="1">
-        <v>1.904761904761898</v>
+        <v>-3.8834951456310538</v>
       </c>
       <c r="O263" s="1">
-        <v>-20.942202338771374</v>
+        <v>-5.2144169776083817</v>
       </c>
       <c r="P263" s="1">
-        <v>1.435478006120873</v>
+        <v>-9.6227513043867816</v>
       </c>
       <c r="Q263" s="1">
-        <v>-3.8191580620877201</v>
+        <v>-1.7198341394584813</v>
       </c>
       <c r="R263" s="1">
-        <v>-1.0850832047256846</v>
+        <v>-0.5108425738784218</v>
       </c>
       <c r="S263" s="1">
-        <v>61.315789473684205</v>
+        <v>18.348623853211009</v>
       </c>
       <c r="T263" s="1">
-        <v>3.773584905660381</v>
+        <v>-8.1818181818181852</v>
       </c>
       <c r="U263" s="1">
-        <v>20.279720279720284</v>
+        <v>-1.8181818181818117</v>
       </c>
     </row>
     <row r="264" spans="1:21" x14ac:dyDescent="0.3">
@@ -17651,55 +17654,55 @@
         <v>33</v>
       </c>
       <c r="E265">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F265">
         <v>2.5</v>
       </c>
       <c r="G265" s="1">
-        <v>-8.0357142857142883</v>
+        <v>3.773584905660381</v>
       </c>
       <c r="H265" s="1">
-        <v>10.796915167095104</v>
+        <v>-0.76468548693574134</v>
       </c>
       <c r="I265" s="1">
-        <v>-169.92287917737789</v>
+        <v>-148.24634034472041</v>
       </c>
       <c r="J265" s="1">
-        <v>1.2089007620510992</v>
+        <v>5.9308077458519595</v>
       </c>
       <c r="K265" s="1">
-        <v>4.3859649122807012</v>
+        <v>-29.292929292929298</v>
       </c>
       <c r="L265" s="1">
-        <v>4.5796989571422255</v>
+        <v>-4.5340041699398395</v>
       </c>
       <c r="M265" s="1">
-        <v>0.72894054446455525</v>
+        <v>5.1422299992189897</v>
       </c>
       <c r="N265" s="1">
-        <v>-3.8834951456310538</v>
+        <v>4.0623642604943395</v>
       </c>
       <c r="O265" s="1">
-        <v>-5.2144169776083817</v>
+        <v>-15.848230296460773</v>
       </c>
       <c r="P265" s="1">
-        <v>-9.6227513043867816</v>
+        <v>-17.384552589681167</v>
       </c>
       <c r="Q265" s="1">
-        <v>-1.7198341394584813</v>
+        <v>12.99156940612769</v>
       </c>
       <c r="R265" s="1">
-        <v>-0.5108425738784218</v>
+        <v>3.8599058893141049</v>
       </c>
       <c r="S265" s="1">
-        <v>18.348623853211009</v>
+        <v>22.638254418058811</v>
       </c>
       <c r="T265" s="1">
-        <v>-8.1818181818181852</v>
+        <v>11.627906976744185</v>
       </c>
       <c r="U265" s="1">
-        <v>-1.8181818181818117</v>
+        <v>14.285714285714278</v>
       </c>
     </row>
     <row r="266" spans="1:21" x14ac:dyDescent="0.3">
@@ -17905,61 +17908,61 @@
         <v>24</v>
       </c>
       <c r="C269" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D269" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E269">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F269">
-        <v>50</v>
+        <v>2.5</v>
       </c>
       <c r="G269" s="1">
-        <v>100</v>
+        <v>-9.7087378640776691</v>
       </c>
       <c r="H269" s="1">
-        <v>13.881748071979432</v>
+        <v>-25.704225352112694</v>
       </c>
       <c r="I269" s="1">
-        <v>-200.77120822622103</v>
+        <v>-201.93905817174519</v>
       </c>
       <c r="J269" s="1">
-        <v>0.76076528516956354</v>
+        <v>9.2242953700632437</v>
       </c>
       <c r="K269" s="1">
-        <v>-2.6315789473684115</v>
+        <v>-3.7639877924720166</v>
       </c>
       <c r="L269" s="1">
-        <v>0.65434636264678436</v>
+        <v>-6.6570029296441895</v>
       </c>
       <c r="M269" s="1">
-        <v>-1.9341089270194425</v>
+        <v>5.4513963725893237</v>
       </c>
       <c r="N269" s="1">
-        <v>-2.9126213592232904</v>
+        <v>-23.857868020304565</v>
       </c>
       <c r="O269" s="1">
-        <v>-1.2655302107569988</v>
+        <v>-55.501205415376887</v>
       </c>
       <c r="P269" s="1">
-        <v>-12.687876569726837</v>
+        <v>6.5059194945309633</v>
       </c>
       <c r="Q269" s="1">
-        <v>1.6044383350860454</v>
+        <v>5.8633938590116923</v>
       </c>
       <c r="R269" s="1">
-        <v>3.0565488323859791</v>
+        <v>7.6254746615990161</v>
       </c>
       <c r="S269" s="1">
-        <v>69.082568807339442</v>
+        <v>-23.964868255959864</v>
       </c>
       <c r="T269" s="1">
-        <v>-14.545454545454543</v>
+        <v>-112.5</v>
       </c>
       <c r="U269" s="1">
-        <v>2.7272727272727337</v>
+        <v>-36.255924170616126</v>
       </c>
     </row>
     <row r="270" spans="1:21" x14ac:dyDescent="0.3">
@@ -18035,61 +18038,61 @@
         <v>24</v>
       </c>
       <c r="C271" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D271" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E271">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F271">
         <v>2.5</v>
       </c>
       <c r="G271" s="1">
-        <v>3.773584905660381</v>
+        <v>-4.3788187372708549</v>
       </c>
       <c r="H271" s="1">
-        <v>-0.76468548693574134</v>
+        <v>4.5115521775546066</v>
       </c>
       <c r="I271" s="1">
-        <v>-148.24634034472041</v>
+        <v>-86.801131291559443</v>
       </c>
       <c r="J271" s="1">
-        <v>5.9308077458519595</v>
+        <v>-3.3260542753818645</v>
       </c>
       <c r="K271" s="1">
-        <v>-29.292929292929298</v>
+        <v>-6.9915254237287918</v>
       </c>
       <c r="L271" s="1">
-        <v>-4.5340041699398395</v>
+        <v>-20.019934778201215</v>
       </c>
       <c r="M271" s="1">
-        <v>5.1422299992189897</v>
+        <v>-1.3440692897956057</v>
       </c>
       <c r="N271" s="1">
-        <v>4.0623642604943395</v>
+        <v>-3.9006938051243565</v>
       </c>
       <c r="O271" s="1">
-        <v>-15.848230296460773</v>
+        <v>-10.696814878370438</v>
       </c>
       <c r="P271" s="1">
-        <v>-17.384552589681167</v>
+        <v>-6.5618923757731116</v>
       </c>
       <c r="Q271" s="1">
-        <v>12.99156940612769</v>
+        <v>1.2883671952913144E-2</v>
       </c>
       <c r="R271" s="1">
-        <v>3.8599058893141049</v>
+        <v>2.9848028599048217</v>
       </c>
       <c r="S271" s="1">
-        <v>22.638254418058811</v>
+        <v>-7.0569685747549995</v>
       </c>
       <c r="T271" s="1">
-        <v>11.627906976744185</v>
+        <v>-3.771551724137931</v>
       </c>
       <c r="U271" s="1">
-        <v>14.285714285714278</v>
+        <v>-6.0924369747898979</v>
       </c>
     </row>
     <row r="272" spans="1:21" x14ac:dyDescent="0.3">
@@ -18292,64 +18295,64 @@
         <v>30</v>
       </c>
       <c r="B275" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C275" t="s">
         <v>29</v>
       </c>
       <c r="D275" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E275">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F275">
-        <v>50</v>
+        <v>2.5</v>
       </c>
       <c r="G275" s="1">
-        <v>100</v>
+        <v>-1.3157894736842251</v>
       </c>
       <c r="H275" s="1">
-        <v>-12.440094360727217</v>
+        <v>-20.474777448071212</v>
       </c>
       <c r="I275" s="1">
-        <v>-156.57997152440109</v>
+        <v>8.1818181818181852</v>
       </c>
       <c r="J275" s="1">
-        <v>5.0619937099927323</v>
+        <v>3.8665301308595086</v>
       </c>
       <c r="K275" s="1">
-        <v>-44.612794612794623</v>
+        <v>10.792079207920791</v>
       </c>
       <c r="L275" s="1">
-        <v>-10.850939672126819</v>
+        <v>1.1404143791261487</v>
       </c>
       <c r="M275" s="1">
-        <v>4.1960599300553376</v>
+        <v>2.4547043098087129</v>
       </c>
       <c r="N275" s="1">
-        <v>0.3398085402496645</v>
+        <v>1.886792452830182</v>
       </c>
       <c r="O275" s="1">
-        <v>-13.098599865302992</v>
+        <v>-26.007492786978997</v>
       </c>
       <c r="P275" s="1">
-        <v>-24.938915695370437</v>
+        <v>2.0194451619125795</v>
       </c>
       <c r="Q275" s="1">
-        <v>3.8656227532704377</v>
+        <v>-7.8641476376106638</v>
       </c>
       <c r="R275" s="1">
-        <v>7.4701613757346967</v>
+        <v>5.3797168219531768</v>
       </c>
       <c r="S275" s="1">
-        <v>72.778760284250382</v>
+        <v>-1.3636363636363547</v>
       </c>
       <c r="T275" s="1">
-        <v>11.369509043927662</v>
+        <v>14.728682170542637</v>
       </c>
       <c r="U275" s="1">
-        <v>16.79894179894179</v>
+        <v>12.173913043478263</v>
       </c>
     </row>
     <row r="276" spans="1:21" x14ac:dyDescent="0.3">
@@ -18422,64 +18425,64 @@
         <v>30</v>
       </c>
       <c r="B277" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C277" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D277" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E277">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F277">
         <v>2.5</v>
       </c>
       <c r="G277" s="1">
-        <v>-9.7087378640776691</v>
+        <v>9.0395480225988578</v>
       </c>
       <c r="H277" s="1">
-        <v>-25.704225352112694</v>
+        <v>-3.7956918283775205</v>
       </c>
       <c r="I277" s="1">
-        <v>-201.93905817174519</v>
+        <v>38.663171690694625</v>
       </c>
       <c r="J277" s="1">
-        <v>9.2242953700632437</v>
+        <v>5.9962283630395135</v>
       </c>
       <c r="K277" s="1">
-        <v>-3.7639877924720166</v>
+        <v>22.140608604407131</v>
       </c>
       <c r="L277" s="1">
-        <v>-6.6570029296441895</v>
+        <v>18.518713638713095</v>
       </c>
       <c r="M277" s="1">
-        <v>5.4513963725893237</v>
+        <v>1.4825410384617692</v>
       </c>
       <c r="N277" s="1">
-        <v>-23.857868020304565</v>
+        <v>5.1867219917012441</v>
       </c>
       <c r="O277" s="1">
-        <v>-55.501205415376887</v>
+        <v>10.578487685093716</v>
       </c>
       <c r="P277" s="1">
-        <v>6.5059194945309633</v>
+        <v>22.150808257725949</v>
       </c>
       <c r="Q277" s="1">
-        <v>5.8633938590116923</v>
+        <v>1.1205231639809532</v>
       </c>
       <c r="R277" s="1">
-        <v>7.6254746615990161</v>
+        <v>9.5987854038923732</v>
       </c>
       <c r="S277" s="1">
-        <v>-23.964868255959864</v>
+        <v>7.3672806067172232</v>
       </c>
       <c r="T277" s="1">
-        <v>-112.5</v>
+        <v>3.1187122736418385</v>
       </c>
       <c r="U277" s="1">
-        <v>-36.255924170616126</v>
+        <v>-2.1233569261880594</v>
       </c>
     </row>
     <row r="278" spans="1:21" x14ac:dyDescent="0.3">
@@ -18682,7 +18685,7 @@
         <v>30</v>
       </c>
       <c r="B281" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C281" t="s">
         <v>34</v>
@@ -18691,55 +18694,55 @@
         <v>33</v>
       </c>
       <c r="E281">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="F281">
-        <v>50</v>
+        <v>2.5</v>
       </c>
       <c r="G281" s="1">
-        <v>100</v>
+        <v>16.737739872068239</v>
       </c>
       <c r="H281" s="1">
-        <v>-33.450704225352112</v>
+        <v>-7.8785444967583391</v>
       </c>
       <c r="I281" s="1">
-        <v>-165.0969529085873</v>
+        <v>-20.979020979020977</v>
       </c>
       <c r="J281" s="1">
-        <v>7.6828338989347751</v>
+        <v>12.544592697601473</v>
       </c>
       <c r="K281" s="1">
-        <v>6.2054933875890077</v>
+        <v>-4.7619047619047619</v>
       </c>
       <c r="L281" s="1">
-        <v>7.150698594546804</v>
+        <v>3.4715215331136884</v>
       </c>
       <c r="M281" s="1">
-        <v>-8.1811001105762511</v>
+        <v>8.560002161289356</v>
       </c>
       <c r="N281" s="1">
-        <v>1.6243654822335041</v>
+        <v>9.0099009900990108</v>
       </c>
       <c r="O281" s="1">
-        <v>-63.915841986997783</v>
+        <v>8.4393113658034071</v>
       </c>
       <c r="P281" s="1">
-        <v>-1.6170550202942138</v>
+        <v>-2.2201997266655931</v>
       </c>
       <c r="Q281" s="1">
-        <v>3.0708943367496198</v>
+        <v>1.9281025665527363</v>
       </c>
       <c r="R281" s="1">
-        <v>5.9529448806588663</v>
+        <v>6.5431667474364037</v>
       </c>
       <c r="S281" s="1">
-        <v>56.963613550815545</v>
+        <v>8.6956521739130554</v>
       </c>
       <c r="T281" s="1">
-        <v>-30.000000000000004</v>
+        <v>12.11211211211212</v>
       </c>
       <c r="U281" s="1">
-        <v>-18.483412322274891</v>
+        <v>6.1165048543689391</v>
       </c>
     </row>
     <row r="282" spans="1:21" x14ac:dyDescent="0.3">
@@ -18812,7 +18815,7 @@
         <v>30</v>
       </c>
       <c r="B283" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C283" t="s">
         <v>34</v>
@@ -18821,55 +18824,55 @@
         <v>33</v>
       </c>
       <c r="E283">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="F283">
         <v>2.5</v>
       </c>
       <c r="G283" s="1">
-        <v>-4.3788187372708549</v>
+        <v>-1.2790697674418745</v>
       </c>
       <c r="H283" s="1">
-        <v>4.5115521775546066</v>
+        <v>11.063608949299805</v>
       </c>
       <c r="I283" s="1">
-        <v>-86.801131291559443</v>
+        <v>21.145833333333329</v>
       </c>
       <c r="J283" s="1">
-        <v>-3.3260542753818645</v>
+        <v>1.84160398908636</v>
       </c>
       <c r="K283" s="1">
-        <v>-6.9915254237287918</v>
+        <v>-11.464968152866241</v>
       </c>
       <c r="L283" s="1">
-        <v>-20.019934778201215</v>
+        <v>7.5519975748013479</v>
       </c>
       <c r="M283" s="1">
-        <v>-1.3440692897956057</v>
+        <v>7.9437504672347226</v>
       </c>
       <c r="N283" s="1">
-        <v>-3.9006938051243565</v>
+        <v>4.0196078431372566</v>
       </c>
       <c r="O283" s="1">
-        <v>-10.696814878370438</v>
+        <v>4.2726419095599883</v>
       </c>
       <c r="P283" s="1">
-        <v>-6.5618923757731116</v>
+        <v>1.8477878949511877</v>
       </c>
       <c r="Q283" s="1">
-        <v>1.2883671952913144E-2</v>
+        <v>7.1339389867098957</v>
       </c>
       <c r="R283" s="1">
-        <v>2.9848028599048217</v>
+        <v>6.692959296121046</v>
       </c>
       <c r="S283" s="1">
-        <v>-7.0569685747549995</v>
+        <v>3.6954087346024647</v>
       </c>
       <c r="T283" s="1">
-        <v>-3.771551724137931</v>
+        <v>4.6078431372548909</v>
       </c>
       <c r="U283" s="1">
-        <v>-6.0924369747898979</v>
+        <v>-8.8987764182424787</v>
       </c>
     </row>
     <row r="284" spans="1:21" x14ac:dyDescent="0.3">
@@ -19072,64 +19075,64 @@
         <v>30</v>
       </c>
       <c r="B287" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C287" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D287" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E287">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="F287">
-        <v>50</v>
+        <v>2.5</v>
       </c>
       <c r="G287" s="1">
-        <v>100</v>
+        <v>9.243697478991594</v>
       </c>
       <c r="H287" s="1">
-        <v>-12.686537961672192</v>
+        <v>-3.8809727848494013</v>
       </c>
       <c r="I287" s="1">
-        <v>-86.358332390147609</v>
+        <v>8.9523809523809472</v>
       </c>
       <c r="J287" s="1">
-        <v>-1.1967188278310199</v>
+        <v>9.8684069035279798</v>
       </c>
       <c r="K287" s="1">
-        <v>-11.228813559322029</v>
+        <v>1.9230769230769333</v>
       </c>
       <c r="L287" s="1">
-        <v>-69.871584098266894</v>
+        <v>9.9747645812055961</v>
       </c>
       <c r="M287" s="1">
-        <v>4.4113440975976008</v>
+        <v>6.1895336800307774</v>
       </c>
       <c r="N287" s="1">
-        <v>9.970961340269449</v>
+        <v>9.603960396039593</v>
       </c>
       <c r="O287" s="1">
-        <v>-6.6687530638687749</v>
+        <v>1.7115090687810277</v>
       </c>
       <c r="P287" s="1">
-        <v>-5.9798714388780798</v>
+        <v>9.8714678245410958</v>
       </c>
       <c r="Q287" s="1">
-        <v>0.48547618105729523</v>
+        <v>4.3190162017510616</v>
       </c>
       <c r="R287" s="1">
-        <v>9.6552514853675984</v>
+        <v>12.470480481310533</v>
       </c>
       <c r="S287" s="1">
-        <v>58.836203015048625</v>
+        <v>5.6701030927834948</v>
       </c>
       <c r="T287" s="1">
-        <v>-30.387931034482751</v>
+        <v>11.504424778761067</v>
       </c>
       <c r="U287" s="1">
-        <v>-20.79831932773109</v>
+        <v>13.942307692307702</v>
       </c>
     </row>
     <row r="288" spans="1:21" x14ac:dyDescent="0.3">
@@ -19205,61 +19208,61 @@
         <v>25</v>
       </c>
       <c r="C289" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D289" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E289">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="F289">
         <v>2.5</v>
       </c>
       <c r="G289" s="1">
-        <v>-1.3157894736842251</v>
+        <v>0.96153846153845812</v>
       </c>
       <c r="H289" s="1">
-        <v>-20.474777448071212</v>
+        <v>1.8240625254369436</v>
       </c>
       <c r="I289" s="1">
-        <v>8.1818181818181852</v>
+        <v>-58.222456456418428</v>
       </c>
       <c r="J289" s="1">
-        <v>3.8665301308595086</v>
+        <v>1.0092236403371355</v>
       </c>
       <c r="K289" s="1">
-        <v>10.792079207920791</v>
+        <v>5.3571428571428541</v>
       </c>
       <c r="L289" s="1">
-        <v>1.1404143791261487</v>
+        <v>-10.878585712512981</v>
       </c>
       <c r="M289" s="1">
-        <v>2.4547043098087129</v>
+        <v>-4.2301450764709365</v>
       </c>
       <c r="N289" s="1">
-        <v>1.886792452830182</v>
+        <v>6.5763587728246362</v>
       </c>
       <c r="O289" s="1">
-        <v>-26.007492786978997</v>
+        <v>-16.774815034638557</v>
       </c>
       <c r="P289" s="1">
-        <v>2.0194451619125795</v>
+        <v>-13.001733946967633</v>
       </c>
       <c r="Q289" s="1">
-        <v>-7.8641476376106638</v>
+        <v>-3.2442077662523312</v>
       </c>
       <c r="R289" s="1">
-        <v>5.3797168219531768</v>
+        <v>-2.457277047795376</v>
       </c>
       <c r="S289" s="1">
-        <v>-1.3636363636363547</v>
+        <v>17.50852898094044</v>
       </c>
       <c r="T289" s="1">
-        <v>14.728682170542637</v>
+        <v>9.0654205607476541</v>
       </c>
       <c r="U289" s="1">
-        <v>12.173913043478263</v>
+        <v>0.93457943925233322</v>
       </c>
     </row>
     <row r="290" spans="1:21" x14ac:dyDescent="0.3">
@@ -19468,58 +19471,58 @@
         <v>29</v>
       </c>
       <c r="D293" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E293">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="F293">
-        <v>50</v>
+        <v>2.5</v>
       </c>
       <c r="G293" s="1">
-        <v>100</v>
+        <v>22.477876106194696</v>
       </c>
       <c r="H293" s="1">
-        <v>-21.958456973293764</v>
+        <v>-21.794197251242185</v>
       </c>
       <c r="I293" s="1">
-        <v>0</v>
+        <v>-11.565006365315311</v>
       </c>
       <c r="J293" s="1">
-        <v>-2.5693272078938345</v>
+        <v>13.716399438975317</v>
       </c>
       <c r="K293" s="1">
-        <v>-19.801980198019802</v>
+        <v>5.6451612903225898</v>
       </c>
       <c r="L293" s="1">
-        <v>-14.864270130244092</v>
+        <v>3.0056561029805615</v>
       </c>
       <c r="M293" s="1">
-        <v>0.24200369809760461</v>
+        <v>13.093574269626732</v>
       </c>
       <c r="N293" s="1">
-        <v>6.3207547169811322</v>
+        <v>7.2758506520558868</v>
       </c>
       <c r="O293" s="1">
-        <v>23.214846511211306</v>
+        <v>26.207728360545126</v>
       </c>
       <c r="P293" s="1">
-        <v>-2.7080558395182317</v>
+        <v>7.6123793808446196</v>
       </c>
       <c r="Q293" s="1">
-        <v>-11.873835831705563</v>
+        <v>17.136025539025741</v>
       </c>
       <c r="R293" s="1">
-        <v>6.0444462262815106</v>
+        <v>11.176439147773186</v>
       </c>
       <c r="S293" s="1">
-        <v>57.5</v>
+        <v>17.699262902076793</v>
       </c>
       <c r="T293" s="1">
-        <v>13.953488372093027</v>
+        <v>12.068965517241383</v>
       </c>
       <c r="U293" s="1">
-        <v>-4.3478260869565215</v>
+        <v>23.816793893129766</v>
       </c>
     </row>
     <row r="294" spans="1:21" x14ac:dyDescent="0.3">
@@ -19592,64 +19595,64 @@
         <v>30</v>
       </c>
       <c r="B295" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C295" t="s">
         <v>29</v>
       </c>
       <c r="D295" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E295">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="F295">
         <v>2.5</v>
       </c>
       <c r="G295" s="1">
-        <v>9.0395480225988578</v>
+        <v>15.151515151515149</v>
       </c>
       <c r="H295" s="1">
-        <v>-3.7956918283775205</v>
+        <v>-12.348029580216297</v>
       </c>
       <c r="I295" s="1">
-        <v>38.663171690694625</v>
+        <v>6.1165048543689391</v>
       </c>
       <c r="J295" s="1">
-        <v>5.9962283630395135</v>
+        <v>9.5146509681028846</v>
       </c>
       <c r="K295" s="1">
-        <v>22.140608604407131</v>
+        <v>-14.093959731543622</v>
       </c>
       <c r="L295" s="1">
-        <v>18.518713638713095</v>
+        <v>8.5179120848144212</v>
       </c>
       <c r="M295" s="1">
-        <v>1.4825410384617692</v>
+        <v>6.9341871283158589</v>
       </c>
       <c r="N295" s="1">
-        <v>5.1867219917012441</v>
+        <v>7.1287128712871173</v>
       </c>
       <c r="O295" s="1">
-        <v>10.578487685093716</v>
+        <v>2.7202436273364845</v>
       </c>
       <c r="P295" s="1">
-        <v>22.150808257725949</v>
+        <v>-2.6599981932630796</v>
       </c>
       <c r="Q295" s="1">
-        <v>1.1205231639809532</v>
+        <v>1.6381813069751441</v>
       </c>
       <c r="R295" s="1">
-        <v>9.5987854038923732</v>
+        <v>12.249303342192352</v>
       </c>
       <c r="S295" s="1">
-        <v>7.3672806067172232</v>
+        <v>4.5893719806763169</v>
       </c>
       <c r="T295" s="1">
-        <v>3.1187122736418385</v>
+        <v>12.941176470588223</v>
       </c>
       <c r="U295" s="1">
-        <v>-2.1233569261880594</v>
+        <v>6.7999999999999972</v>
       </c>
     </row>
     <row r="296" spans="1:21" x14ac:dyDescent="0.3">
@@ -19852,64 +19855,64 @@
         <v>30</v>
       </c>
       <c r="B299" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C299" t="s">
         <v>29</v>
       </c>
       <c r="D299" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E299">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="F299">
-        <v>50</v>
+        <v>2.5</v>
       </c>
       <c r="G299" s="1">
-        <v>100</v>
+        <v>-0.3042596348884497</v>
       </c>
       <c r="H299" s="1">
-        <v>-12.479162218419372</v>
+        <v>15.979753201807711</v>
       </c>
       <c r="I299" s="1">
-        <v>-21.363040629095675</v>
+        <v>7.9646017699115061</v>
       </c>
       <c r="J299" s="1">
-        <v>4.297453847755631</v>
+        <v>10.194634887542684</v>
       </c>
       <c r="K299" s="1">
-        <v>-4.5120671563483894</v>
+        <v>-11.764705882352953</v>
       </c>
       <c r="L299" s="1">
-        <v>1.7576164306387867</v>
+        <v>6.2875089877849373</v>
       </c>
       <c r="M299" s="1">
-        <v>4.7524027208177495</v>
+        <v>4.4875749090798056</v>
       </c>
       <c r="N299" s="1">
-        <v>4.4605809128630671</v>
+        <v>7.4074074074074137</v>
       </c>
       <c r="O299" s="1">
-        <v>18.028829387445825</v>
+        <v>9.506804451193922</v>
       </c>
       <c r="P299" s="1">
-        <v>12.746932223442821</v>
+        <v>4.3077880518948515</v>
       </c>
       <c r="Q299" s="1">
-        <v>-2.1040526175867229</v>
+        <v>3.8673690349227758</v>
       </c>
       <c r="R299" s="1">
-        <v>11.404269724828092</v>
+        <v>4.5237724313719712</v>
       </c>
       <c r="S299" s="1">
-        <v>51.462621885157091</v>
+        <v>11.328527291452124</v>
       </c>
       <c r="T299" s="1">
-        <v>3.7223340040241371</v>
+        <v>17.386091127098325</v>
       </c>
       <c r="U299" s="1">
-        <v>5.8645096056622856</v>
+        <v>-7.7908217716115313</v>
       </c>
     </row>
     <row r="300" spans="1:21" x14ac:dyDescent="0.3">
@@ -19982,64 +19985,64 @@
         <v>30</v>
       </c>
       <c r="B301" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C301" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D301" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E301">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="F301">
         <v>2.5</v>
       </c>
       <c r="G301" s="1">
-        <v>16.737739872068239</v>
+        <v>11.090909090909095</v>
       </c>
       <c r="H301" s="1">
-        <v>-7.8785444967583391</v>
+        <v>21.425614181091561</v>
       </c>
       <c r="I301" s="1">
-        <v>-20.979020979020977</v>
+        <v>4.753966201161397</v>
       </c>
       <c r="J301" s="1">
-        <v>12.544592697601473</v>
+        <v>7.2652144986766745</v>
       </c>
       <c r="K301" s="1">
-        <v>-4.7619047619047619</v>
+        <v>0.82644628099173267</v>
       </c>
       <c r="L301" s="1">
-        <v>3.4715215331136884</v>
+        <v>4.937843645641161</v>
       </c>
       <c r="M301" s="1">
-        <v>8.560002161289356</v>
+        <v>-5.0794191664783854</v>
       </c>
       <c r="N301" s="1">
-        <v>9.0099009900990108</v>
+        <v>-3.0205889555745378</v>
       </c>
       <c r="O301" s="1">
-        <v>8.4393113658034071</v>
+        <v>5.5460340239856993</v>
       </c>
       <c r="P301" s="1">
-        <v>-2.2201997266655931</v>
+        <v>12.456033357368735</v>
       </c>
       <c r="Q301" s="1">
-        <v>1.9281025665527363</v>
+        <v>11.164033807488057</v>
       </c>
       <c r="R301" s="1">
-        <v>6.5431667474364037</v>
+        <v>8.1167648843840965</v>
       </c>
       <c r="S301" s="1">
-        <v>8.6956521739130554</v>
+        <v>16.163267867477117</v>
       </c>
       <c r="T301" s="1">
-        <v>12.11211211211212</v>
+        <v>12.396694214876034</v>
       </c>
       <c r="U301" s="1">
-        <v>6.1165048543689391</v>
+        <v>3.3613445378151288</v>
       </c>
     </row>
     <row r="302" spans="1:21" x14ac:dyDescent="0.3">
@@ -20242,64 +20245,64 @@
         <v>30</v>
       </c>
       <c r="B305" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C305" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D305" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E305">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="F305">
-        <v>50</v>
+        <v>2.5</v>
       </c>
       <c r="G305" s="1">
-        <v>53.731343283582099</v>
+        <v>-18.736383442265801</v>
       </c>
       <c r="H305" s="1">
-        <v>9.5402099674485719</v>
+        <v>1.2567666545210794</v>
       </c>
       <c r="I305" s="1">
-        <v>-29.790209790209772</v>
+        <v>-4.7313712821136349</v>
       </c>
       <c r="J305" s="1">
-        <v>5.6564730426535288</v>
+        <v>3.6051457859857332</v>
       </c>
       <c r="K305" s="1">
-        <v>8.7619047619047628</v>
+        <v>-3.8095238095238129</v>
       </c>
       <c r="L305" s="1">
-        <v>-1.1166282037287534</v>
+        <v>9.1262687518658225</v>
       </c>
       <c r="M305" s="1">
-        <v>-3.2084239367123657</v>
+        <v>16.760592435026382</v>
       </c>
       <c r="N305" s="1">
-        <v>1.8811881188118764</v>
+        <v>4.2964117499670156</v>
       </c>
       <c r="O305" s="1">
-        <v>4.0517473182334891</v>
+        <v>6.1585734783081394</v>
       </c>
       <c r="P305" s="1">
-        <v>-8.376789271377401</v>
+        <v>6.3395623411148794</v>
       </c>
       <c r="Q305" s="1">
-        <v>1.5600041162870326</v>
+        <v>-0.70577528846154336</v>
       </c>
       <c r="R305" s="1">
-        <v>4.088276829976202</v>
+        <v>8.5149430446317815</v>
       </c>
       <c r="S305" s="1">
-        <v>32.6644370122631</v>
+        <v>17.047457228894107</v>
       </c>
       <c r="T305" s="1">
-        <v>-3.1031031031031082</v>
+        <v>5.4054054054054026</v>
       </c>
       <c r="U305" s="1">
-        <v>0.97087378640778077</v>
+        <v>9.7014925373134364</v>
       </c>
     </row>
     <row r="306" spans="1:21" x14ac:dyDescent="0.3">
@@ -20372,64 +20375,64 @@
         <v>30</v>
       </c>
       <c r="B307" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C307" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D307" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E307">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="F307">
         <v>2.5</v>
       </c>
       <c r="G307" s="1">
-        <v>-1.2790697674418745</v>
+        <v>-0.60679611650484144</v>
       </c>
       <c r="H307" s="1">
-        <v>11.063608949299805</v>
+        <v>18.226851062904938</v>
       </c>
       <c r="I307" s="1">
-        <v>21.145833333333329</v>
+        <v>10.909090909090903</v>
       </c>
       <c r="J307" s="1">
-        <v>1.84160398908636</v>
+        <v>2.9273302631325699</v>
       </c>
       <c r="K307" s="1">
-        <v>-11.464968152866241</v>
+        <v>24.758064516129032</v>
       </c>
       <c r="L307" s="1">
-        <v>7.5519975748013479</v>
+        <v>16.477917087001771</v>
       </c>
       <c r="M307" s="1">
-        <v>7.9437504672347226</v>
+        <v>6.1058948073426471</v>
       </c>
       <c r="N307" s="1">
-        <v>4.0196078431372566</v>
+        <v>13.302752293577992</v>
       </c>
       <c r="O307" s="1">
-        <v>4.2726419095599883</v>
+        <v>3.5293161878260926</v>
       </c>
       <c r="P307" s="1">
-        <v>1.8477878949511877</v>
+        <v>10.375023695720945</v>
       </c>
       <c r="Q307" s="1">
-        <v>7.1339389867098957</v>
+        <v>6.5202300496342822</v>
       </c>
       <c r="R307" s="1">
-        <v>6.692959296121046</v>
+        <v>3.4407576232789236</v>
       </c>
       <c r="S307" s="1">
-        <v>3.6954087346024647</v>
+        <v>6.3784311095771793</v>
       </c>
       <c r="T307" s="1">
-        <v>4.6078431372548909</v>
+        <v>13.079299691040179</v>
       </c>
       <c r="U307" s="1">
-        <v>-8.8987764182424787</v>
+        <v>15.000000000000007</v>
       </c>
     </row>
     <row r="308" spans="1:21" x14ac:dyDescent="0.3">
@@ -20632,64 +20635,64 @@
         <v>30</v>
       </c>
       <c r="B311" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C311" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D311" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E311">
-        <v>29</v>
+        <v>85</v>
       </c>
       <c r="F311">
-        <v>50</v>
+        <v>2.5</v>
       </c>
       <c r="G311" s="1">
-        <v>29.418604651162784</v>
+        <v>0.83532219570406063</v>
       </c>
       <c r="H311" s="1">
-        <v>7.0157544007456938</v>
+        <v>-2.6703977510423011</v>
       </c>
       <c r="I311" s="1">
-        <v>2.8124999999999956</v>
+        <v>15.396637861624784</v>
       </c>
       <c r="J311" s="1">
-        <v>5.5262280628181584</v>
+        <v>24.723267425515623</v>
       </c>
       <c r="K311" s="1">
-        <v>-11.464968152866241</v>
+        <v>17.524752475247521</v>
       </c>
       <c r="L311" s="1">
-        <v>6.1507922880850492</v>
+        <v>23.293532180650864</v>
       </c>
       <c r="M311" s="1">
-        <v>11.098420324032329</v>
+        <v>12.546316209203528</v>
       </c>
       <c r="N311" s="1">
-        <v>5.9803921568627398</v>
+        <v>10.089728552984328</v>
       </c>
       <c r="O311" s="1">
-        <v>2.0748791848360644</v>
+        <v>12.22215081230356</v>
       </c>
       <c r="P311" s="1">
-        <v>6.3204956579611284</v>
+        <v>8.8037783707529265</v>
       </c>
       <c r="Q311" s="1">
-        <v>6.2035431319463124</v>
+        <v>17.532444854311969</v>
       </c>
       <c r="R311" s="1">
-        <v>15.081922608587812</v>
+        <v>11.793169403076529</v>
       </c>
       <c r="S311" s="1">
-        <v>21.05263157894737</v>
+        <v>30.646695066109171</v>
       </c>
       <c r="T311" s="1">
-        <v>-1.9607843137255008</v>
+        <v>10.865384615384624</v>
       </c>
       <c r="U311" s="1">
-        <v>-15.684093437152391</v>
+        <v>2.7027027027026933</v>
       </c>
     </row>
     <row r="312" spans="1:21" x14ac:dyDescent="0.3">
@@ -20762,64 +20765,64 @@
         <v>30</v>
       </c>
       <c r="B313" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C313" t="s">
         <v>29</v>
       </c>
       <c r="D313" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E313">
-        <v>30</v>
+        <v>92</v>
       </c>
       <c r="F313">
         <v>2.5</v>
       </c>
       <c r="G313" s="1">
-        <v>9.243697478991594</v>
+        <v>34.250000000000007</v>
       </c>
       <c r="H313" s="1">
-        <v>-3.8809727848494013</v>
+        <v>29.126085770527524</v>
       </c>
       <c r="I313" s="1">
-        <v>8.9523809523809472</v>
+        <v>-14.529355700207979</v>
       </c>
       <c r="J313" s="1">
-        <v>9.8684069035279798</v>
+        <v>6.821220218715788</v>
       </c>
       <c r="K313" s="1">
-        <v>1.9230769230769333</v>
+        <v>14.179104477611942</v>
       </c>
       <c r="L313" s="1">
-        <v>9.9747645812055961</v>
+        <v>70.90906448572845</v>
       </c>
       <c r="M313" s="1">
-        <v>6.1895336800307774</v>
+        <v>10.424815462774013</v>
       </c>
       <c r="N313" s="1">
-        <v>9.603960396039593</v>
+        <v>8.7776590902283669</v>
       </c>
       <c r="O313" s="1">
-        <v>1.7115090687810277</v>
+        <v>4.8996557744921461</v>
       </c>
       <c r="P313" s="1">
-        <v>9.8714678245410958</v>
+        <v>12.983249149147758</v>
       </c>
       <c r="Q313" s="1">
-        <v>4.3190162017510616</v>
+        <v>-23.864425468729763</v>
       </c>
       <c r="R313" s="1">
-        <v>12.470480481310533</v>
+        <v>26.028657486194582</v>
       </c>
       <c r="S313" s="1">
-        <v>5.6701030927834948</v>
+        <v>5.6752177820614262</v>
       </c>
       <c r="T313" s="1">
-        <v>11.504424778761067</v>
+        <v>-56.25</v>
       </c>
       <c r="U313" s="1">
-        <v>13.942307692307702</v>
+        <v>11.66666666666667</v>
       </c>
     </row>
     <row r="314" spans="1:21" x14ac:dyDescent="0.3">
@@ -21022,64 +21025,64 @@
         <v>30</v>
       </c>
       <c r="B317" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C317" t="s">
         <v>29</v>
       </c>
       <c r="D317" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E317">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="F317">
-        <v>50</v>
+        <v>2.5</v>
       </c>
       <c r="G317" s="1">
-        <v>65.12605042016807</v>
+        <v>29.074074074074076</v>
       </c>
       <c r="H317" s="1">
-        <v>-14.036696670517586</v>
+        <v>-6.8009424309226434</v>
       </c>
       <c r="I317" s="1">
-        <v>7.3333333333333295</v>
+        <v>14.750430839779545</v>
       </c>
       <c r="J317" s="1">
-        <v>4.785121079058035</v>
+        <v>3.0086580949609987</v>
       </c>
       <c r="K317" s="1">
-        <v>4.9038461538461515</v>
+        <v>1.5267175572519029</v>
       </c>
       <c r="L317" s="1">
-        <v>8.4785838825563626</v>
+        <v>72.176407296570659</v>
       </c>
       <c r="M317" s="1">
-        <v>4.8246020089589008</v>
+        <v>12.126319886921499</v>
       </c>
       <c r="N317" s="1">
-        <v>2.9702970297029601</v>
+        <v>2.4938460043180295</v>
       </c>
       <c r="O317" s="1">
-        <v>-0.68759590822525929</v>
+        <v>-3.7775798121030975</v>
       </c>
       <c r="P317" s="1">
-        <v>8.6906059014639592</v>
+        <v>11.493081890329586</v>
       </c>
       <c r="Q317" s="1">
-        <v>0.6576757458780168</v>
+        <v>6.9322250121734115</v>
       </c>
       <c r="R317" s="1">
-        <v>8.6070641385488447</v>
+        <v>16.376034741193539</v>
       </c>
       <c r="S317" s="1">
-        <v>40.515463917525778</v>
+        <v>18.827107626415195</v>
       </c>
       <c r="T317" s="1">
-        <v>7.9646017699115061</v>
+        <v>17.368421052631582</v>
       </c>
       <c r="U317" s="1">
-        <v>7.4038461538461497</v>
+        <v>14.503816793893133</v>
       </c>
     </row>
     <row r="318" spans="1:21" x14ac:dyDescent="0.3">
@@ -21152,64 +21155,64 @@
         <v>30</v>
       </c>
       <c r="B319" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C319" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D319" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E319">
-        <v>36</v>
+        <v>99</v>
       </c>
       <c r="F319">
         <v>2.5</v>
       </c>
       <c r="G319" s="1">
-        <v>0.96153846153845812</v>
+        <v>28.214285714285712</v>
       </c>
       <c r="H319" s="1">
-        <v>1.8240625254369436</v>
+        <v>-0.82680801867793663</v>
       </c>
       <c r="I319" s="1">
-        <v>-58.222456456418428</v>
+        <v>10.950028949972111</v>
       </c>
       <c r="J319" s="1">
-        <v>1.0092236403371355</v>
+        <v>14.917627673908916</v>
       </c>
       <c r="K319" s="1">
-        <v>5.3571428571428541</v>
+        <v>0.78740157480315276</v>
       </c>
       <c r="L319" s="1">
-        <v>-10.878585712512981</v>
+        <v>25.351127540846729</v>
       </c>
       <c r="M319" s="1">
-        <v>-4.2301450764709365</v>
+        <v>15.599479715474304</v>
       </c>
       <c r="N319" s="1">
-        <v>6.5763587728246362</v>
+        <v>19.729602770053678</v>
       </c>
       <c r="O319" s="1">
-        <v>-16.774815034638557</v>
+        <v>7.7787754873152632</v>
       </c>
       <c r="P319" s="1">
-        <v>-13.001733946967633</v>
+        <v>8.9520655103927371</v>
       </c>
       <c r="Q319" s="1">
-        <v>-3.2442077662523312</v>
+        <v>15.836311350850822</v>
       </c>
       <c r="R319" s="1">
-        <v>-2.457277047795376</v>
+        <v>17.512268631149585</v>
       </c>
       <c r="S319" s="1">
-        <v>17.50852898094044</v>
+        <v>9.9669993636547201</v>
       </c>
       <c r="T319" s="1">
-        <v>9.0654205607476541</v>
+        <v>5.7692307692307656</v>
       </c>
       <c r="U319" s="1">
-        <v>0.93457943925233322</v>
+        <v>17.352941176470583</v>
       </c>
     </row>
     <row r="320" spans="1:21" x14ac:dyDescent="0.3">
@@ -21412,64 +21415,64 @@
         <v>30</v>
       </c>
       <c r="B323" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C323" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D323" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E323">
-        <v>36</v>
+        <v>113</v>
       </c>
       <c r="F323">
-        <v>50</v>
+        <v>2.5</v>
       </c>
       <c r="G323" s="1">
-        <v>47.21153846153846</v>
+        <v>31.633714880332978</v>
       </c>
       <c r="H323" s="1">
-        <v>11.669296573807072</v>
+        <v>16.489296884844624</v>
       </c>
       <c r="I323" s="1">
-        <v>-59.977234823403542</v>
+        <v>7.6598608790018856</v>
       </c>
       <c r="J323" s="1">
-        <v>3.1503984286928044</v>
+        <v>11.225031156795792</v>
       </c>
       <c r="K323" s="1">
-        <v>-17.857142857142858</v>
+        <v>24.15094339622642</v>
       </c>
       <c r="L323" s="1">
-        <v>-15.752981460730453</v>
+        <v>23.509523938487543</v>
       </c>
       <c r="M323" s="1">
-        <v>-2.766564239783051</v>
+        <v>12.585689345876117</v>
       </c>
       <c r="N323" s="1">
-        <v>-2.0278589145989532</v>
+        <v>16.801760431122652</v>
       </c>
       <c r="O323" s="1">
-        <v>-5.7048421019024635</v>
+        <v>15.663081479736995</v>
       </c>
       <c r="P323" s="1">
-        <v>-17.807642452485585</v>
+        <v>15.071558148423426</v>
       </c>
       <c r="Q323" s="1">
-        <v>-3.5967402464750733</v>
+        <v>11.0733650103692</v>
       </c>
       <c r="R323" s="1">
-        <v>-5.9083536806106514</v>
+        <v>15.377587553141106</v>
       </c>
       <c r="S323" s="1">
-        <v>29.386470079598325</v>
+        <v>25.576923076923077</v>
       </c>
       <c r="T323" s="1">
-        <v>-1.8691588785046829</v>
+        <v>15.871559633027527</v>
       </c>
       <c r="U323" s="1">
-        <v>2.8037383177569994</v>
+        <v>22.222222222222225</v>
       </c>
     </row>
     <row r="324" spans="1:21" x14ac:dyDescent="0.3">
@@ -21542,64 +21545,64 @@
         <v>30</v>
       </c>
       <c r="B325" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C325" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D325" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E325">
-        <v>42</v>
+        <v>120</v>
       </c>
       <c r="F325">
         <v>2.5</v>
       </c>
       <c r="G325" s="1">
-        <v>22.477876106194696</v>
+        <v>6.5693430656934204</v>
       </c>
       <c r="H325" s="1">
-        <v>-21.794197251242185</v>
+        <v>21.469331862030945</v>
       </c>
       <c r="I325" s="1">
-        <v>-11.565006365315311</v>
+        <v>-15.835077454737796</v>
       </c>
       <c r="J325" s="1">
-        <v>13.716399438975317</v>
+        <v>3.4602884076565492</v>
       </c>
       <c r="K325" s="1">
-        <v>5.6451612903225898</v>
+        <v>14.049586776859499</v>
       </c>
       <c r="L325" s="1">
-        <v>3.0056561029805615</v>
+        <v>63.766948215261223</v>
       </c>
       <c r="M325" s="1">
-        <v>13.093574269626732</v>
+        <v>32.298230923288024</v>
       </c>
       <c r="N325" s="1">
-        <v>7.2758506520558868</v>
+        <v>5.2637564697332797</v>
       </c>
       <c r="O325" s="1">
-        <v>26.207728360545126</v>
+        <v>0.88320643187484582</v>
       </c>
       <c r="P325" s="1">
-        <v>7.6123793808446196</v>
+        <v>5.5877735522179872</v>
       </c>
       <c r="Q325" s="1">
-        <v>17.136025539025741</v>
+        <v>18.943622699650302</v>
       </c>
       <c r="R325" s="1">
-        <v>11.176439147773186</v>
+        <v>8.8725882589018905</v>
       </c>
       <c r="S325" s="1">
-        <v>17.699262902076793</v>
+        <v>-12.998077805909565</v>
       </c>
       <c r="T325" s="1">
-        <v>12.068965517241383</v>
+        <v>22.11864406779662</v>
       </c>
       <c r="U325" s="1">
-        <v>23.816793893129766</v>
+        <v>3.1746031746031775</v>
       </c>
     </row>
     <row r="326" spans="1:21" x14ac:dyDescent="0.3">
@@ -21802,64 +21805,64 @@
         <v>30</v>
       </c>
       <c r="B329" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C329" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D329" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E329">
-        <v>42</v>
+        <v>126</v>
       </c>
       <c r="F329">
-        <v>50</v>
+        <v>2.5</v>
       </c>
       <c r="G329" s="1">
-        <v>53.451327433628329</v>
+        <v>16.666666666666668</v>
       </c>
       <c r="H329" s="1">
-        <v>-24.381812375590673</v>
+        <v>15.946430690037413</v>
       </c>
       <c r="I329" s="1">
-        <v>-14.26280458028382</v>
+        <v>-100.21127578293681</v>
       </c>
       <c r="J329" s="1">
-        <v>6.0873078383682451</v>
+        <v>13.228857943908903</v>
       </c>
       <c r="K329" s="1">
-        <v>10.483870967741939</v>
+        <v>-13.592233009708723</v>
       </c>
       <c r="L329" s="1">
-        <v>-11.222624466875606</v>
+        <v>51.100675561797175</v>
       </c>
       <c r="M329" s="1">
-        <v>6.7424557222097734</v>
+        <v>12.838991063745867</v>
       </c>
       <c r="N329" s="1">
-        <v>5.4604348222762669</v>
+        <v>-10.391204507485345</v>
       </c>
       <c r="O329" s="1">
-        <v>18.390293413659553</v>
+        <v>-0.18370369950166177</v>
       </c>
       <c r="P329" s="1">
-        <v>10.931614500034922</v>
+        <v>-15.135983880256132</v>
       </c>
       <c r="Q329" s="1">
-        <v>11.837628930142314</v>
+        <v>9.8487164969732977</v>
       </c>
       <c r="R329" s="1">
-        <v>7.3719879515103193</v>
+        <v>3.9120154195448538</v>
       </c>
       <c r="S329" s="1">
-        <v>35.474720501356693</v>
+        <v>13.167816840911437</v>
       </c>
       <c r="T329" s="1">
-        <v>4.3103448275862073</v>
+        <v>11.304347826086962</v>
       </c>
       <c r="U329" s="1">
-        <v>16.030534351145036</v>
+        <v>8.3333333333333321</v>
       </c>
     </row>
     <row r="330" spans="1:21" x14ac:dyDescent="0.3">
@@ -21932,7 +21935,7 @@
         <v>30</v>
       </c>
       <c r="B331" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="C331" t="s">
         <v>29</v>
@@ -21941,55 +21944,55 @@
         <v>35</v>
       </c>
       <c r="E331">
-        <v>43</v>
+        <v>127</v>
       </c>
       <c r="F331">
         <v>2.5</v>
       </c>
       <c r="G331" s="1">
-        <v>15.151515151515149</v>
+        <v>7.9019073569482297</v>
       </c>
       <c r="H331" s="1">
-        <v>-12.348029580216297</v>
+        <v>14.156176776825536</v>
       </c>
       <c r="I331" s="1">
-        <v>6.1165048543689391</v>
+        <v>8.6400782189226177</v>
       </c>
       <c r="J331" s="1">
-        <v>9.5146509681028846</v>
+        <v>11.616904339957685</v>
       </c>
       <c r="K331" s="1">
-        <v>-14.093959731543622</v>
+        <v>-0.94339622641509102</v>
       </c>
       <c r="L331" s="1">
-        <v>8.5179120848144212</v>
+        <v>29.379372774062713</v>
       </c>
       <c r="M331" s="1">
-        <v>6.9341871283158589</v>
+        <v>12.067357017596606</v>
       </c>
       <c r="N331" s="1">
-        <v>7.1287128712871173</v>
+        <v>9.5003198983918775</v>
       </c>
       <c r="O331" s="1">
-        <v>2.7202436273364845</v>
+        <v>7.3684465417796527</v>
       </c>
       <c r="P331" s="1">
-        <v>-2.6599981932630796</v>
+        <v>4.0109213644374364</v>
       </c>
       <c r="Q331" s="1">
-        <v>1.6381813069751441</v>
+        <v>19.882646586574513</v>
       </c>
       <c r="R331" s="1">
-        <v>12.249303342192352</v>
+        <v>17.838971865909532</v>
       </c>
       <c r="S331" s="1">
-        <v>4.5893719806763169</v>
+        <v>-21.160054060380073</v>
       </c>
       <c r="T331" s="1">
-        <v>12.941176470588223</v>
+        <v>15.412844036697244</v>
       </c>
       <c r="U331" s="1">
-        <v>6.7999999999999972</v>
+        <v>6.4220183486238636</v>
       </c>
     </row>
     <row r="332" spans="1:21" x14ac:dyDescent="0.3">
@@ -22192,7 +22195,7 @@
         <v>30</v>
       </c>
       <c r="B335" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="C335" t="s">
         <v>29</v>
@@ -22201,55 +22204,55 @@
         <v>35</v>
       </c>
       <c r="E335">
-        <v>43</v>
+        <v>142</v>
       </c>
       <c r="F335">
-        <v>50</v>
+        <v>2.5</v>
       </c>
       <c r="G335" s="1">
-        <v>62.354312354312356</v>
+        <v>21.874999999999996</v>
       </c>
       <c r="H335" s="1">
-        <v>-4.7333784294040697</v>
+        <v>16.325073795067652</v>
       </c>
       <c r="I335" s="1">
-        <v>4.5631067961165108</v>
+        <v>10.985978119274966</v>
       </c>
       <c r="J335" s="1">
-        <v>9.6402758026197333</v>
+        <v>13.521101658507428</v>
       </c>
       <c r="K335" s="1">
-        <v>-4.4742729306487741</v>
+        <v>-2.4340770791075075</v>
       </c>
       <c r="L335" s="1">
-        <v>7.9298088854952908</v>
+        <v>26.314783542392469</v>
       </c>
       <c r="M335" s="1">
-        <v>5.7011880249169238</v>
+        <v>6.378174984405816</v>
       </c>
       <c r="N335" s="1">
-        <v>5.4455445544554353</v>
+        <v>17.028724470418581</v>
       </c>
       <c r="O335" s="1">
-        <v>4.2137258120981018</v>
+        <v>3.4056062706377865</v>
       </c>
       <c r="P335" s="1">
-        <v>-3.0183194894878014</v>
+        <v>9.8521267526814071</v>
       </c>
       <c r="Q335" s="1">
-        <v>-5.7025156352844153</v>
+        <v>14.1271221847962</v>
       </c>
       <c r="R335" s="1">
-        <v>10.968786149985982</v>
+        <v>9.5599010082904972</v>
       </c>
       <c r="S335" s="1">
-        <v>24.999999999999996</v>
+        <v>54.981013113053933</v>
       </c>
       <c r="T335" s="1">
-        <v>14.705882352941178</v>
+        <v>3.8293216630197091</v>
       </c>
       <c r="U335" s="1">
-        <v>-5</v>
+        <v>9.649122807017541</v>
       </c>
     </row>
     <row r="336" spans="1:21" x14ac:dyDescent="0.3">
@@ -22322,64 +22325,64 @@
         <v>30</v>
       </c>
       <c r="B337" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="C337" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D337" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E337">
-        <v>57</v>
+        <v>148</v>
       </c>
       <c r="F337">
         <v>2.5</v>
       </c>
       <c r="G337" s="1">
-        <v>-0.3042596348884497</v>
+        <v>38.721804511278194</v>
       </c>
       <c r="H337" s="1">
-        <v>15.979753201807711</v>
+        <v>1.6099461769504189</v>
       </c>
       <c r="I337" s="1">
-        <v>7.9646017699115061</v>
+        <v>-32.030308835050995</v>
       </c>
       <c r="J337" s="1">
-        <v>10.194634887542684</v>
+        <v>-18.878288525348228</v>
       </c>
       <c r="K337" s="1">
-        <v>-11.764705882352953</v>
+        <v>3.4722222222222223</v>
       </c>
       <c r="L337" s="1">
-        <v>6.2875089877849373</v>
+        <v>-7.50466745822765</v>
       </c>
       <c r="M337" s="1">
-        <v>4.4875749090798056</v>
+        <v>14.179371347332351</v>
       </c>
       <c r="N337" s="1">
-        <v>7.4074074074074137</v>
+        <v>-7.2122114011544367</v>
       </c>
       <c r="O337" s="1">
-        <v>9.506804451193922</v>
+        <v>12.328726143692432</v>
       </c>
       <c r="P337" s="1">
-        <v>4.3077880518948515</v>
+        <v>-9.2549770111207721</v>
       </c>
       <c r="Q337" s="1">
-        <v>3.8673690349227758</v>
+        <v>-31.877041988105347</v>
       </c>
       <c r="R337" s="1">
-        <v>4.5237724313719712</v>
+        <v>11.802665924220515</v>
       </c>
       <c r="S337" s="1">
-        <v>11.328527291452124</v>
+        <v>45.455733669659317</v>
       </c>
       <c r="T337" s="1">
-        <v>17.386091127098325</v>
+        <v>2.2727272727272649</v>
       </c>
       <c r="U337" s="1">
-        <v>-7.7908217716115313</v>
+        <v>12.643678160919539</v>
       </c>
     </row>
     <row r="338" spans="1:21" x14ac:dyDescent="0.3">
@@ -22582,64 +22585,64 @@
         <v>30</v>
       </c>
       <c r="B341" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="C341" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D341" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E341">
-        <v>57</v>
+        <v>154</v>
       </c>
       <c r="F341">
-        <v>50</v>
-      </c>
-      <c r="G341" s="1">
-        <v>50.709939148073012</v>
+        <v>2.5</v>
+      </c>
+      <c r="G341" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="H341" s="1">
-        <v>15.695760568970718</v>
+        <v>6.3725677728714798</v>
       </c>
       <c r="I341" s="1">
-        <v>9.7345132743362957</v>
+        <v>-33.22007031576856</v>
       </c>
       <c r="J341" s="1">
-        <v>4.4309864998343</v>
+        <v>1.5539269591014728</v>
       </c>
       <c r="K341" s="1">
-        <v>-16.666666666666679</v>
+        <v>-3.2786885245901671</v>
       </c>
       <c r="L341" s="1">
-        <v>7.6998874469154917</v>
+        <v>10.432399260333597</v>
       </c>
       <c r="M341" s="1">
-        <v>6.8757915370988014</v>
+        <v>5.6320802083774533</v>
       </c>
       <c r="N341" s="1">
-        <v>10.648148148148151</v>
+        <v>-8.3228093953704632E-2</v>
       </c>
       <c r="O341" s="1">
-        <v>8.9628479227734648</v>
+        <v>-77.841296186673645</v>
       </c>
       <c r="P341" s="1">
-        <v>7.1545676445222535</v>
+        <v>0.6849410628318815</v>
       </c>
       <c r="Q341" s="1">
-        <v>12.082083825724611</v>
+        <v>-6.7082997072445112</v>
       </c>
       <c r="R341" s="1">
-        <v>8.2921123277516635</v>
+        <v>3.1790047119904843</v>
       </c>
       <c r="S341" s="1">
-        <v>28.733264675592181</v>
+        <v>68.277545903157801</v>
       </c>
       <c r="T341" s="1">
-        <v>17.026378896882495</v>
+        <v>11.363636363636365</v>
       </c>
       <c r="U341" s="1">
-        <v>12.806830309498393</v>
+        <v>11.194029850746269</v>
       </c>
     </row>
     <row r="342" spans="1:21" x14ac:dyDescent="0.3">
@@ -22712,64 +22715,64 @@
         <v>30</v>
       </c>
       <c r="B343" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C343" t="s">
         <v>29</v>
       </c>
       <c r="D343" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E343">
-        <v>64</v>
+        <v>1</v>
       </c>
       <c r="F343">
-        <v>2.5</v>
+        <v>50</v>
       </c>
       <c r="G343" s="1">
-        <v>11.090909090909095</v>
+        <v>100</v>
       </c>
       <c r="H343" s="1">
-        <v>21.425614181091561</v>
+        <v>15.789473684210513</v>
       </c>
       <c r="I343" s="1">
-        <v>4.753966201161397</v>
+        <v>-8.6642599277978203</v>
       </c>
       <c r="J343" s="1">
-        <v>7.2652144986766745</v>
+        <v>-1.1756715966961206</v>
       </c>
       <c r="K343" s="1">
-        <v>0.82644628099173267</v>
+        <v>5.4545454545454515</v>
       </c>
       <c r="L343" s="1">
-        <v>4.937843645641161</v>
+        <v>2.2257326566507274</v>
       </c>
       <c r="M343" s="1">
-        <v>-5.0794191664783854</v>
+        <v>-0.38303354394105016</v>
       </c>
       <c r="N343" s="1">
-        <v>-3.0205889555745378</v>
+        <v>1.904761904761898</v>
       </c>
       <c r="O343" s="1">
-        <v>5.5460340239856993</v>
+        <v>-20.942202338771374</v>
       </c>
       <c r="P343" s="1">
-        <v>12.456033357368735</v>
+        <v>1.435478006120873</v>
       </c>
       <c r="Q343" s="1">
-        <v>11.164033807488057</v>
+        <v>-3.8191580620877201</v>
       </c>
       <c r="R343" s="1">
-        <v>8.1167648843840965</v>
+        <v>-1.0850832047256846</v>
       </c>
       <c r="S343" s="1">
-        <v>16.163267867477117</v>
+        <v>61.315789473684205</v>
       </c>
       <c r="T343" s="1">
-        <v>12.396694214876034</v>
+        <v>3.773584905660381</v>
       </c>
       <c r="U343" s="1">
-        <v>3.3613445378151288</v>
+        <v>20.279720279720284</v>
       </c>
     </row>
     <row r="344" spans="1:21" x14ac:dyDescent="0.3">
@@ -22972,7 +22975,7 @@
         <v>30</v>
       </c>
       <c r="B347" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C347" t="s">
         <v>29</v>
@@ -22981,55 +22984,55 @@
         <v>33</v>
       </c>
       <c r="E347">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="F347">
         <v>50</v>
       </c>
       <c r="G347" s="1">
-        <v>46.545454545454547</v>
+        <v>100</v>
       </c>
       <c r="H347" s="1">
-        <v>17.012983578318817</v>
+        <v>13.881748071979432</v>
       </c>
       <c r="I347" s="1">
-        <v>-3.8907131929957082</v>
+        <v>-200.77120822622103</v>
       </c>
       <c r="J347" s="1">
-        <v>-3.4274323917093223E-2</v>
+        <v>0.76076528516956354</v>
       </c>
       <c r="K347" s="1">
-        <v>0.82644628099173267</v>
+        <v>-2.6315789473684115</v>
       </c>
       <c r="L347" s="1">
-        <v>-6.3742378416370711</v>
+        <v>0.65434636264678436</v>
       </c>
       <c r="M347" s="1">
-        <v>-9.3038623915548566</v>
+        <v>-1.9341089270194425</v>
       </c>
       <c r="N347" s="1">
-        <v>-1.3398164151404601</v>
+        <v>-2.9126213592232904</v>
       </c>
       <c r="O347" s="1">
-        <v>1.1153902655131738</v>
+        <v>-1.2655302107569988</v>
       </c>
       <c r="P347" s="1">
-        <v>6.3785677745702438</v>
+        <v>-12.687876569726837</v>
       </c>
       <c r="Q347" s="1">
-        <v>-0.55907088020355167</v>
+        <v>1.6044383350860454</v>
       </c>
       <c r="R347" s="1">
-        <v>4.438269077347333</v>
+        <v>3.0565488323859791</v>
       </c>
       <c r="S347" s="1">
-        <v>40.542180808106068</v>
+        <v>69.082568807339442</v>
       </c>
       <c r="T347" s="1">
-        <v>4.95867768595041</v>
+        <v>-14.545454545454543</v>
       </c>
       <c r="U347" s="1">
-        <v>-5.0420168067226863</v>
+        <v>2.7272727272727337</v>
       </c>
     </row>
     <row r="348" spans="1:21" x14ac:dyDescent="0.3">
@@ -23102,7 +23105,7 @@
         <v>30</v>
       </c>
       <c r="B349" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C349" t="s">
         <v>29</v>
@@ -23111,55 +23114,55 @@
         <v>33</v>
       </c>
       <c r="E349">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="F349">
-        <v>2.5</v>
+        <v>50</v>
       </c>
       <c r="G349" s="1">
-        <v>-18.736383442265801</v>
+        <v>100</v>
       </c>
       <c r="H349" s="1">
-        <v>1.2567666545210794</v>
+        <v>-12.440094360727217</v>
       </c>
       <c r="I349" s="1">
-        <v>-4.7313712821136349</v>
+        <v>-156.57997152440109</v>
       </c>
       <c r="J349" s="1">
-        <v>3.6051457859857332</v>
+        <v>5.0619937099927323</v>
       </c>
       <c r="K349" s="1">
-        <v>-3.8095238095238129</v>
+        <v>-44.612794612794623</v>
       </c>
       <c r="L349" s="1">
-        <v>9.1262687518658225</v>
+        <v>-10.850939672126819</v>
       </c>
       <c r="M349" s="1">
-        <v>16.760592435026382</v>
+        <v>4.1960599300553376</v>
       </c>
       <c r="N349" s="1">
-        <v>4.2964117499670156</v>
+        <v>0.3398085402496645</v>
       </c>
       <c r="O349" s="1">
-        <v>6.1585734783081394</v>
+        <v>-13.098599865302992</v>
       </c>
       <c r="P349" s="1">
-        <v>6.3395623411148794</v>
+        <v>-24.938915695370437</v>
       </c>
       <c r="Q349" s="1">
-        <v>-0.70577528846154336</v>
+        <v>3.8656227532704377</v>
       </c>
       <c r="R349" s="1">
-        <v>8.5149430446317815</v>
+        <v>7.4701613757346967</v>
       </c>
       <c r="S349" s="1">
-        <v>17.047457228894107</v>
+        <v>72.778760284250382</v>
       </c>
       <c r="T349" s="1">
-        <v>5.4054054054054026</v>
+        <v>11.369509043927662</v>
       </c>
       <c r="U349" s="1">
-        <v>9.7014925373134364</v>
+        <v>16.79894179894179</v>
       </c>
     </row>
     <row r="350" spans="1:21" x14ac:dyDescent="0.3">
@@ -23362,64 +23365,64 @@
         <v>30</v>
       </c>
       <c r="B353" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C353" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D353" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E353">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="F353">
         <v>50</v>
       </c>
       <c r="G353" s="1">
-        <v>33.006535947712415</v>
+        <v>100</v>
       </c>
       <c r="H353" s="1">
-        <v>1.662497400305931</v>
+        <v>-33.450704225352112</v>
       </c>
       <c r="I353" s="1">
-        <v>26.721031980241634</v>
+        <v>-165.0969529085873</v>
       </c>
       <c r="J353" s="1">
-        <v>-5.2851091285743959</v>
+        <v>7.6828338989347751</v>
       </c>
       <c r="K353" s="1">
-        <v>-4.7619047619047619</v>
+        <v>6.2054933875890077</v>
       </c>
       <c r="L353" s="1">
-        <v>-2.4552566529149709</v>
+        <v>7.150698594546804</v>
       </c>
       <c r="M353" s="1">
-        <v>-0.54532822019669602</v>
+        <v>-8.1811001105762511</v>
       </c>
       <c r="N353" s="1">
-        <v>0.51701431601065551</v>
+        <v>1.6243654822335041</v>
       </c>
       <c r="O353" s="1">
-        <v>-6.8045337605753682</v>
+        <v>-63.915841986997783</v>
       </c>
       <c r="P353" s="1">
-        <v>12.091338484304766</v>
+        <v>-1.6170550202942138</v>
       </c>
       <c r="Q353" s="1">
-        <v>-1.3932728588825638</v>
+        <v>3.0708943367496198</v>
       </c>
       <c r="R353" s="1">
-        <v>0.95746253141306392</v>
+        <v>5.9529448806588663</v>
       </c>
       <c r="S353" s="1">
-        <v>16.405010112995111</v>
+        <v>56.963613550815545</v>
       </c>
       <c r="T353" s="1">
-        <v>0</v>
+        <v>-30.000000000000004</v>
       </c>
       <c r="U353" s="1">
-        <v>10.447761194029853</v>
+        <v>-18.483412322274891</v>
       </c>
     </row>
     <row r="354" spans="1:21" x14ac:dyDescent="0.3">
@@ -23492,64 +23495,64 @@
         <v>30</v>
       </c>
       <c r="B355" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C355" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D355" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E355">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="F355">
-        <v>2.5</v>
+        <v>50</v>
       </c>
       <c r="G355" s="1">
-        <v>-0.60679611650484144</v>
+        <v>100</v>
       </c>
       <c r="H355" s="1">
-        <v>18.226851062904938</v>
+        <v>-12.686537961672192</v>
       </c>
       <c r="I355" s="1">
-        <v>10.909090909090903</v>
+        <v>-86.358332390147609</v>
       </c>
       <c r="J355" s="1">
-        <v>2.9273302631325699</v>
+        <v>-1.1967188278310199</v>
       </c>
       <c r="K355" s="1">
-        <v>24.758064516129032</v>
+        <v>-11.228813559322029</v>
       </c>
       <c r="L355" s="1">
-        <v>16.477917087001771</v>
+        <v>-69.871584098266894</v>
       </c>
       <c r="M355" s="1">
-        <v>6.1058948073426471</v>
+        <v>4.4113440975976008</v>
       </c>
       <c r="N355" s="1">
-        <v>13.302752293577992</v>
+        <v>9.970961340269449</v>
       </c>
       <c r="O355" s="1">
-        <v>3.5293161878260926</v>
+        <v>-6.6687530638687749</v>
       </c>
       <c r="P355" s="1">
-        <v>10.375023695720945</v>
+        <v>-5.9798714388780798</v>
       </c>
       <c r="Q355" s="1">
-        <v>6.5202300496342822</v>
+        <v>0.48547618105729523</v>
       </c>
       <c r="R355" s="1">
-        <v>3.4407576232789236</v>
+        <v>9.6552514853675984</v>
       </c>
       <c r="S355" s="1">
-        <v>6.3784311095771793</v>
+        <v>58.836203015048625</v>
       </c>
       <c r="T355" s="1">
-        <v>13.079299691040179</v>
+        <v>-30.387931034482751</v>
       </c>
       <c r="U355" s="1">
-        <v>15.000000000000007</v>
+        <v>-20.79831932773109</v>
       </c>
     </row>
     <row r="356" spans="1:21" x14ac:dyDescent="0.3">
@@ -23752,7 +23755,7 @@
         <v>30</v>
       </c>
       <c r="B359" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C359" t="s">
         <v>29</v>
@@ -23761,55 +23764,55 @@
         <v>35</v>
       </c>
       <c r="E359">
-        <v>71</v>
+        <v>15</v>
       </c>
       <c r="F359">
         <v>50</v>
       </c>
       <c r="G359" s="1">
-        <v>48.179611650485441</v>
+        <v>100</v>
       </c>
       <c r="H359" s="1">
-        <v>23.419524385492416</v>
+        <v>-21.958456973293764</v>
       </c>
       <c r="I359" s="1">
-        <v>10.181818181818175</v>
+        <v>0</v>
       </c>
       <c r="J359" s="1">
-        <v>1.5727599219254442</v>
+        <v>-2.5693272078938345</v>
       </c>
       <c r="K359" s="1">
-        <v>1.6129032258064602</v>
+        <v>-19.801980198019802</v>
       </c>
       <c r="L359" s="1">
-        <v>5.5690479940736815</v>
+        <v>-14.864270130244092</v>
       </c>
       <c r="M359" s="1">
-        <v>0.13472116199864989</v>
+        <v>0.24200369809760461</v>
       </c>
       <c r="N359" s="1">
-        <v>12.660550458715603</v>
+        <v>6.3207547169811322</v>
       </c>
       <c r="O359" s="1">
-        <v>-1.3241576244461708</v>
+        <v>23.214846511211306</v>
       </c>
       <c r="P359" s="1">
-        <v>8.6663364882646405</v>
+        <v>-2.7080558395182317</v>
       </c>
       <c r="Q359" s="1">
-        <v>5.9340292716969989</v>
+        <v>-11.873835831705563</v>
       </c>
       <c r="R359" s="1">
-        <v>7.0401562041533738</v>
+        <v>6.0444462262815106</v>
       </c>
       <c r="S359" s="1">
-        <v>30.835656755117746</v>
+        <v>57.5</v>
       </c>
       <c r="T359" s="1">
-        <v>39.237899073120495</v>
+        <v>13.953488372093027</v>
       </c>
       <c r="U359" s="1">
-        <v>26.666666666666675</v>
+        <v>-4.3478260869565215</v>
       </c>
     </row>
     <row r="360" spans="1:21" x14ac:dyDescent="0.3">
@@ -23882,64 +23885,64 @@
         <v>30</v>
       </c>
       <c r="B361" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C361" t="s">
         <v>29</v>
       </c>
       <c r="D361" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E361">
-        <v>85</v>
+        <v>22</v>
       </c>
       <c r="F361">
-        <v>2.5</v>
+        <v>50</v>
       </c>
       <c r="G361" s="1">
-        <v>0.83532219570406063</v>
+        <v>100</v>
       </c>
       <c r="H361" s="1">
-        <v>-2.6703977510423011</v>
+        <v>-12.479162218419372</v>
       </c>
       <c r="I361" s="1">
-        <v>15.396637861624784</v>
+        <v>-21.363040629095675</v>
       </c>
       <c r="J361" s="1">
-        <v>24.723267425515623</v>
+        <v>4.297453847755631</v>
       </c>
       <c r="K361" s="1">
-        <v>17.524752475247521</v>
+        <v>-4.5120671563483894</v>
       </c>
       <c r="L361" s="1">
-        <v>23.293532180650864</v>
+        <v>1.7576164306387867</v>
       </c>
       <c r="M361" s="1">
-        <v>12.546316209203528</v>
+        <v>4.7524027208177495</v>
       </c>
       <c r="N361" s="1">
-        <v>10.089728552984328</v>
+        <v>4.4605809128630671</v>
       </c>
       <c r="O361" s="1">
-        <v>12.22215081230356</v>
+        <v>18.028829387445825</v>
       </c>
       <c r="P361" s="1">
-        <v>8.8037783707529265</v>
+        <v>12.746932223442821</v>
       </c>
       <c r="Q361" s="1">
-        <v>17.532444854311969</v>
+        <v>-2.1040526175867229</v>
       </c>
       <c r="R361" s="1">
-        <v>11.793169403076529</v>
+        <v>11.404269724828092</v>
       </c>
       <c r="S361" s="1">
-        <v>30.646695066109171</v>
+        <v>51.462621885157091</v>
       </c>
       <c r="T361" s="1">
-        <v>10.865384615384624</v>
+        <v>3.7223340040241371</v>
       </c>
       <c r="U361" s="1">
-        <v>2.7027027027026933</v>
+        <v>5.8645096056622856</v>
       </c>
     </row>
     <row r="362" spans="1:21" x14ac:dyDescent="0.3">
@@ -24142,64 +24145,64 @@
         <v>30</v>
       </c>
       <c r="B365" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C365" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D365" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E365">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="F365">
         <v>50</v>
       </c>
       <c r="G365" s="1">
-        <v>39.140811455847263</v>
+        <v>53.731343283582099</v>
       </c>
       <c r="H365" s="1">
-        <v>13.239460115109472</v>
+        <v>9.5402099674485719</v>
       </c>
       <c r="I365" s="1">
-        <v>2.3416369957330652</v>
+        <v>-29.790209790209772</v>
       </c>
       <c r="J365" s="1">
-        <v>29.320510117936401</v>
+        <v>5.6564730426535288</v>
       </c>
       <c r="K365" s="1">
-        <v>-10.891089108910888</v>
+        <v>8.7619047619047628</v>
       </c>
       <c r="L365" s="1">
-        <v>9.6895856360953729</v>
+        <v>-1.1166282037287534</v>
       </c>
       <c r="M365" s="1">
-        <v>7.2283297851002297</v>
+        <v>-3.2084239367123657</v>
       </c>
       <c r="N365" s="1">
-        <v>8.7975729943756615</v>
+        <v>1.8811881188118764</v>
       </c>
       <c r="O365" s="1">
-        <v>7.7287753134868824</v>
+        <v>4.0517473182334891</v>
       </c>
       <c r="P365" s="1">
-        <v>1.3899248538075564</v>
+        <v>-8.376789271377401</v>
       </c>
       <c r="Q365" s="1">
-        <v>24.758392155487968</v>
+        <v>1.5600041162870326</v>
       </c>
       <c r="R365" s="1">
-        <v>3.0899139937893971</v>
+        <v>4.088276829976202</v>
       </c>
       <c r="S365" s="1">
-        <v>36.359150459036002</v>
+        <v>32.6644370122631</v>
       </c>
       <c r="T365" s="1">
-        <v>17.211538461538471</v>
+        <v>-3.1031031031031082</v>
       </c>
       <c r="U365" s="1">
-        <v>12.432432432432423</v>
+        <v>0.97087378640778077</v>
       </c>
     </row>
     <row r="366" spans="1:21" x14ac:dyDescent="0.3">
@@ -24272,64 +24275,64 @@
         <v>30</v>
       </c>
       <c r="B367" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C367" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D367" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E367">
-        <v>92</v>
+        <v>29</v>
       </c>
       <c r="F367">
-        <v>2.5</v>
+        <v>50</v>
       </c>
       <c r="G367" s="1">
-        <v>34.250000000000007</v>
+        <v>29.418604651162784</v>
       </c>
       <c r="H367" s="1">
-        <v>29.126085770527524</v>
+        <v>7.0157544007456938</v>
       </c>
       <c r="I367" s="1">
-        <v>-14.529355700207979</v>
+        <v>2.8124999999999956</v>
       </c>
       <c r="J367" s="1">
-        <v>6.821220218715788</v>
+        <v>5.5262280628181584</v>
       </c>
       <c r="K367" s="1">
-        <v>14.179104477611942</v>
+        <v>-11.464968152866241</v>
       </c>
       <c r="L367" s="1">
-        <v>70.90906448572845</v>
+        <v>6.1507922880850492</v>
       </c>
       <c r="M367" s="1">
-        <v>10.424815462774013</v>
+        <v>11.098420324032329</v>
       </c>
       <c r="N367" s="1">
-        <v>8.7776590902283669</v>
+        <v>5.9803921568627398</v>
       </c>
       <c r="O367" s="1">
-        <v>4.8996557744921461</v>
+        <v>2.0748791848360644</v>
       </c>
       <c r="P367" s="1">
-        <v>12.983249149147758</v>
+        <v>6.3204956579611284</v>
       </c>
       <c r="Q367" s="1">
-        <v>-23.864425468729763</v>
+        <v>6.2035431319463124</v>
       </c>
       <c r="R367" s="1">
-        <v>26.028657486194582</v>
+        <v>15.081922608587812</v>
       </c>
       <c r="S367" s="1">
-        <v>5.6752177820614262</v>
+        <v>21.05263157894737</v>
       </c>
       <c r="T367" s="1">
-        <v>-56.25</v>
+        <v>-1.9607843137255008</v>
       </c>
       <c r="U367" s="1">
-        <v>11.66666666666667</v>
+        <v>-15.684093437152391</v>
       </c>
     </row>
     <row r="368" spans="1:21" x14ac:dyDescent="0.3">
@@ -24532,64 +24535,64 @@
         <v>30</v>
       </c>
       <c r="B371" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C371" t="s">
         <v>29</v>
       </c>
       <c r="D371" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E371">
-        <v>92</v>
+        <v>30</v>
       </c>
       <c r="F371">
         <v>50</v>
       </c>
       <c r="G371" s="1">
-        <v>64.75</v>
+        <v>65.12605042016807</v>
       </c>
       <c r="H371" s="1">
-        <v>-31.172531672228612</v>
+        <v>-14.036696670517586</v>
       </c>
       <c r="I371" s="1">
-        <v>-48.760362039503576</v>
+        <v>7.3333333333333295</v>
       </c>
       <c r="J371" s="1">
-        <v>-25.878328048769067</v>
+        <v>4.785121079058035</v>
       </c>
       <c r="K371" s="1">
-        <v>-3.7313432835820897</v>
+        <v>4.9038461538461515</v>
       </c>
       <c r="L371" s="1">
-        <v>-30.446323255704296</v>
+        <v>8.4785838825563626</v>
       </c>
       <c r="M371" s="1">
-        <v>2.9755468518967647</v>
+        <v>4.8246020089589008</v>
       </c>
       <c r="N371" s="1">
-        <v>-1.0301243516850336</v>
+        <v>2.9702970297029601</v>
       </c>
       <c r="O371" s="1">
-        <v>-2.7392348718780144</v>
+        <v>-0.68759590822525929</v>
       </c>
       <c r="P371" s="1">
-        <v>10.58502628483202</v>
+        <v>8.6906059014639592</v>
       </c>
       <c r="Q371" s="1">
-        <v>-20.81976356248493</v>
+        <v>0.6576757458780168</v>
       </c>
       <c r="R371" s="1">
-        <v>6.3111520246506423</v>
+        <v>8.6070641385488447</v>
       </c>
       <c r="S371" s="1">
-        <v>48.691514637815416</v>
+        <v>40.515463917525778</v>
       </c>
       <c r="T371" s="1">
-        <v>-74.107142857142847</v>
+        <v>7.9646017699115061</v>
       </c>
       <c r="U371" s="1">
-        <v>-4.9999999999999973</v>
+        <v>7.4038461538461497</v>
       </c>
     </row>
     <row r="372" spans="1:21" x14ac:dyDescent="0.3">
@@ -24662,64 +24665,64 @@
         <v>30</v>
       </c>
       <c r="B373" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C373" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D373" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E373">
-        <v>98</v>
+        <v>36</v>
       </c>
       <c r="F373">
-        <v>2.5</v>
+        <v>50</v>
       </c>
       <c r="G373" s="1">
-        <v>29.074074074074076</v>
+        <v>47.21153846153846</v>
       </c>
       <c r="H373" s="1">
-        <v>-6.8009424309226434</v>
+        <v>11.669296573807072</v>
       </c>
       <c r="I373" s="1">
-        <v>14.750430839779545</v>
+        <v>-59.977234823403542</v>
       </c>
       <c r="J373" s="1">
-        <v>3.0086580949609987</v>
+        <v>3.1503984286928044</v>
       </c>
       <c r="K373" s="1">
-        <v>1.5267175572519029</v>
+        <v>-17.857142857142858</v>
       </c>
       <c r="L373" s="1">
-        <v>72.176407296570659</v>
+        <v>-15.752981460730453</v>
       </c>
       <c r="M373" s="1">
-        <v>12.126319886921499</v>
+        <v>-2.766564239783051</v>
       </c>
       <c r="N373" s="1">
-        <v>2.4938460043180295</v>
+        <v>-2.0278589145989532</v>
       </c>
       <c r="O373" s="1">
-        <v>-3.7775798121030975</v>
+        <v>-5.7048421019024635</v>
       </c>
       <c r="P373" s="1">
-        <v>11.493081890329586</v>
+        <v>-17.807642452485585</v>
       </c>
       <c r="Q373" s="1">
-        <v>6.9322250121734115</v>
+        <v>-3.5967402464750733</v>
       </c>
       <c r="R373" s="1">
-        <v>16.376034741193539</v>
+        <v>-5.9083536806106514</v>
       </c>
       <c r="S373" s="1">
-        <v>18.827107626415195</v>
+        <v>29.386470079598325</v>
       </c>
       <c r="T373" s="1">
-        <v>17.368421052631582</v>
+        <v>-1.8691588785046829</v>
       </c>
       <c r="U373" s="1">
-        <v>14.503816793893133</v>
+        <v>2.8037383177569994</v>
       </c>
     </row>
     <row r="374" spans="1:21" x14ac:dyDescent="0.3">
@@ -24922,7 +24925,7 @@
         <v>30</v>
       </c>
       <c r="B377" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C377" t="s">
         <v>29</v>
@@ -24931,55 +24934,55 @@
         <v>33</v>
       </c>
       <c r="E377">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="F377">
         <v>50</v>
       </c>
       <c r="G377" s="1">
-        <v>77.592592592592595</v>
+        <v>53.451327433628329</v>
       </c>
       <c r="H377" s="1">
-        <v>-4.5154096007960698</v>
+        <v>-24.381812375590673</v>
       </c>
       <c r="I377" s="1">
-        <v>32.364468939966528</v>
+        <v>-14.26280458028382</v>
       </c>
       <c r="J377" s="1">
-        <v>2.2847280945335569</v>
+        <v>6.0873078383682451</v>
       </c>
       <c r="K377" s="1">
-        <v>-12.213740458015266</v>
+        <v>10.483870967741939</v>
       </c>
       <c r="L377" s="1">
-        <v>9.6192835807068864</v>
+        <v>-11.222624466875606</v>
       </c>
       <c r="M377" s="1">
-        <v>-8.4639890254564119</v>
+        <v>6.7424557222097734</v>
       </c>
       <c r="N377" s="1">
-        <v>-12.848731857680818</v>
+        <v>5.4604348222762669</v>
       </c>
       <c r="O377" s="1">
-        <v>-5.0812585325580271</v>
+        <v>18.390293413659553</v>
       </c>
       <c r="P377" s="1">
-        <v>6.7962499411558799</v>
+        <v>10.931614500034922</v>
       </c>
       <c r="Q377" s="1">
-        <v>11.708051053734422</v>
+        <v>11.837628930142314</v>
       </c>
       <c r="R377" s="1">
-        <v>10.606877537239267</v>
+        <v>7.3719879515103193</v>
       </c>
       <c r="S377" s="1">
-        <v>54.226827551063785</v>
+        <v>35.474720501356693</v>
       </c>
       <c r="T377" s="1">
-        <v>4.3859649122807012</v>
+        <v>4.3103448275862073</v>
       </c>
       <c r="U377" s="1">
-        <v>3.8167938931297711</v>
+        <v>16.030534351145036</v>
       </c>
     </row>
     <row r="378" spans="1:21" x14ac:dyDescent="0.3">
@@ -25052,7 +25055,7 @@
         <v>30</v>
       </c>
       <c r="B379" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C379" t="s">
         <v>29</v>
@@ -25061,55 +25064,55 @@
         <v>35</v>
       </c>
       <c r="E379">
-        <v>99</v>
+        <v>43</v>
       </c>
       <c r="F379">
-        <v>2.5</v>
+        <v>50</v>
       </c>
       <c r="G379" s="1">
-        <v>28.214285714285712</v>
+        <v>62.354312354312356</v>
       </c>
       <c r="H379" s="1">
-        <v>-0.82680801867793663</v>
+        <v>-4.7333784294040697</v>
       </c>
       <c r="I379" s="1">
-        <v>10.950028949972111</v>
+        <v>4.5631067961165108</v>
       </c>
       <c r="J379" s="1">
-        <v>14.917627673908916</v>
+        <v>9.6402758026197333</v>
       </c>
       <c r="K379" s="1">
-        <v>0.78740157480315276</v>
+        <v>-4.4742729306487741</v>
       </c>
       <c r="L379" s="1">
-        <v>25.351127540846729</v>
+        <v>7.9298088854952908</v>
       </c>
       <c r="M379" s="1">
-        <v>15.599479715474304</v>
+        <v>5.7011880249169238</v>
       </c>
       <c r="N379" s="1">
-        <v>19.729602770053678</v>
+        <v>5.4455445544554353</v>
       </c>
       <c r="O379" s="1">
-        <v>7.7787754873152632</v>
+        <v>4.2137258120981018</v>
       </c>
       <c r="P379" s="1">
-        <v>8.9520655103927371</v>
+        <v>-3.0183194894878014</v>
       </c>
       <c r="Q379" s="1">
-        <v>15.836311350850822</v>
+        <v>-5.7025156352844153</v>
       </c>
       <c r="R379" s="1">
-        <v>17.512268631149585</v>
+        <v>10.968786149985982</v>
       </c>
       <c r="S379" s="1">
-        <v>9.9669993636547201</v>
+        <v>24.999999999999996</v>
       </c>
       <c r="T379" s="1">
-        <v>5.7692307692307656</v>
+        <v>14.705882352941178</v>
       </c>
       <c r="U379" s="1">
-        <v>17.352941176470583</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="380" spans="1:21" x14ac:dyDescent="0.3">
@@ -25312,7 +25315,7 @@
         <v>30</v>
       </c>
       <c r="B383" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C383" t="s">
         <v>29</v>
@@ -25321,55 +25324,55 @@
         <v>35</v>
       </c>
       <c r="E383">
-        <v>99</v>
+        <v>57</v>
       </c>
       <c r="F383">
         <v>50</v>
       </c>
       <c r="G383" s="1">
-        <v>61.904761904761905</v>
+        <v>50.709939148073012</v>
       </c>
       <c r="H383" s="1">
-        <v>-19.550606257123928</v>
+        <v>15.695760568970718</v>
       </c>
       <c r="I383" s="1">
-        <v>-1.386100088067223</v>
+        <v>9.7345132743362957</v>
       </c>
       <c r="J383" s="1">
-        <v>1.5430455347521295</v>
+        <v>4.4309864998343</v>
       </c>
       <c r="K383" s="1">
-        <v>-11.586051743532051</v>
+        <v>-16.666666666666679</v>
       </c>
       <c r="L383" s="1">
-        <v>6.9246849928859451</v>
+        <v>7.6998874469154917</v>
       </c>
       <c r="M383" s="1">
-        <v>4.6893810050200116E-2</v>
+        <v>6.8757915370988014</v>
       </c>
       <c r="N383" s="1">
-        <v>-4.350039664907162E-2</v>
+        <v>10.648148148148151</v>
       </c>
       <c r="O383" s="1">
-        <v>-6.4344882714734348</v>
+        <v>8.9628479227734648</v>
       </c>
       <c r="P383" s="1">
-        <v>-9.818939222084154</v>
+        <v>7.1545676445222535</v>
       </c>
       <c r="Q383" s="1">
-        <v>7.3396519103064026</v>
+        <v>12.082083825724611</v>
       </c>
       <c r="R383" s="1">
-        <v>0.40168194899612775</v>
+        <v>8.2921123277516635</v>
       </c>
       <c r="S383" s="1">
-        <v>37.676866903079031</v>
+        <v>28.733264675592181</v>
       </c>
       <c r="T383" s="1">
-        <v>21.057692307692303</v>
+        <v>17.026378896882495</v>
       </c>
       <c r="U383" s="1">
-        <v>6.9607843137254823</v>
+        <v>12.806830309498393</v>
       </c>
     </row>
     <row r="384" spans="1:21" x14ac:dyDescent="0.3">
@@ -25442,64 +25445,64 @@
         <v>30</v>
       </c>
       <c r="B385" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C385" t="s">
         <v>29</v>
       </c>
       <c r="D385" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E385">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="F385">
-        <v>2.5</v>
+        <v>50</v>
       </c>
       <c r="G385" s="1">
-        <v>31.633714880332978</v>
+        <v>46.545454545454547</v>
       </c>
       <c r="H385" s="1">
-        <v>16.489296884844624</v>
+        <v>17.012983578318817</v>
       </c>
       <c r="I385" s="1">
-        <v>7.6598608790018856</v>
+        <v>-3.8907131929957082</v>
       </c>
       <c r="J385" s="1">
-        <v>11.225031156795792</v>
+        <v>-3.4274323917093223E-2</v>
       </c>
       <c r="K385" s="1">
-        <v>24.15094339622642</v>
+        <v>0.82644628099173267</v>
       </c>
       <c r="L385" s="1">
-        <v>23.509523938487543</v>
+        <v>-6.3742378416370711</v>
       </c>
       <c r="M385" s="1">
-        <v>12.585689345876117</v>
+        <v>-9.3038623915548566</v>
       </c>
       <c r="N385" s="1">
-        <v>16.801760431122652</v>
+        <v>-1.3398164151404601</v>
       </c>
       <c r="O385" s="1">
-        <v>15.663081479736995</v>
+        <v>1.1153902655131738</v>
       </c>
       <c r="P385" s="1">
-        <v>15.071558148423426</v>
+        <v>6.3785677745702438</v>
       </c>
       <c r="Q385" s="1">
-        <v>11.0733650103692</v>
+        <v>-0.55907088020355167</v>
       </c>
       <c r="R385" s="1">
-        <v>15.377587553141106</v>
+        <v>4.438269077347333</v>
       </c>
       <c r="S385" s="1">
-        <v>25.576923076923077</v>
+        <v>40.542180808106068</v>
       </c>
       <c r="T385" s="1">
-        <v>15.871559633027527</v>
+        <v>4.95867768595041</v>
       </c>
       <c r="U385" s="1">
-        <v>22.222222222222225</v>
+        <v>-5.0420168067226863</v>
       </c>
     </row>
     <row r="386" spans="1:21" x14ac:dyDescent="0.3">
@@ -25702,64 +25705,64 @@
         <v>30</v>
       </c>
       <c r="B389" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C389" t="s">
         <v>29</v>
       </c>
       <c r="D389" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E389">
-        <v>113</v>
+        <v>70</v>
       </c>
       <c r="F389">
         <v>50</v>
       </c>
       <c r="G389" s="1">
-        <v>48.387096774193544</v>
+        <v>33.006535947712415</v>
       </c>
       <c r="H389" s="1">
-        <v>16.077995002928894</v>
+        <v>1.662497400305931</v>
       </c>
       <c r="I389" s="1">
-        <v>15.297664126849131</v>
+        <v>26.721031980241634</v>
       </c>
       <c r="J389" s="1">
-        <v>9.2944321170583901</v>
+        <v>-5.2851091285743959</v>
       </c>
       <c r="K389" s="1">
-        <v>3.773584905660381</v>
+        <v>-4.7619047619047619</v>
       </c>
       <c r="L389" s="1">
-        <v>8.4191254799941291</v>
+        <v>-2.4552566529149709</v>
       </c>
       <c r="M389" s="1">
-        <v>5.4122442068287482</v>
+        <v>-0.54532822019669602</v>
       </c>
       <c r="N389" s="1">
-        <v>17.096461103074201</v>
+        <v>0.51701431601065551</v>
       </c>
       <c r="O389" s="1">
-        <v>14.611798243799317</v>
+        <v>-6.8045337605753682</v>
       </c>
       <c r="P389" s="1">
-        <v>24.232850340135126</v>
+        <v>12.091338484304766</v>
       </c>
       <c r="Q389" s="1">
-        <v>10.491545018553513</v>
+        <v>-1.3932728588825638</v>
       </c>
       <c r="R389" s="1">
-        <v>7.1462695534399572</v>
+        <v>0.95746253141306392</v>
       </c>
       <c r="S389" s="1">
-        <v>40.38461538461538</v>
+        <v>16.405010112995111</v>
       </c>
       <c r="T389" s="1">
-        <v>7.3394495412844103</v>
+        <v>0</v>
       </c>
       <c r="U389" s="1">
-        <v>8.4967320261437944</v>
+        <v>10.447761194029853</v>
       </c>
     </row>
     <row r="390" spans="1:21" x14ac:dyDescent="0.3">
@@ -25832,64 +25835,64 @@
         <v>30</v>
       </c>
       <c r="B391" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C391" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D391" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E391">
-        <v>120</v>
+        <v>71</v>
       </c>
       <c r="F391">
-        <v>2.5</v>
+        <v>50</v>
       </c>
       <c r="G391" s="1">
-        <v>6.5693430656934204</v>
+        <v>48.179611650485441</v>
       </c>
       <c r="H391" s="1">
-        <v>21.469331862030945</v>
+        <v>23.419524385492416</v>
       </c>
       <c r="I391" s="1">
-        <v>-15.835077454737796</v>
+        <v>10.181818181818175</v>
       </c>
       <c r="J391" s="1">
-        <v>3.4602884076565492</v>
+        <v>1.5727599219254442</v>
       </c>
       <c r="K391" s="1">
-        <v>14.049586776859499</v>
+        <v>1.6129032258064602</v>
       </c>
       <c r="L391" s="1">
-        <v>63.766948215261223</v>
+        <v>5.5690479940736815</v>
       </c>
       <c r="M391" s="1">
-        <v>32.298230923288024</v>
+        <v>0.13472116199864989</v>
       </c>
       <c r="N391" s="1">
-        <v>5.2637564697332797</v>
+        <v>12.660550458715603</v>
       </c>
       <c r="O391" s="1">
-        <v>0.88320643187484582</v>
+        <v>-1.3241576244461708</v>
       </c>
       <c r="P391" s="1">
-        <v>5.5877735522179872</v>
+        <v>8.6663364882646405</v>
       </c>
       <c r="Q391" s="1">
-        <v>18.943622699650302</v>
+        <v>5.9340292716969989</v>
       </c>
       <c r="R391" s="1">
-        <v>8.8725882589018905</v>
+        <v>7.0401562041533738</v>
       </c>
       <c r="S391" s="1">
-        <v>-12.998077805909565</v>
+        <v>30.835656755117746</v>
       </c>
       <c r="T391" s="1">
-        <v>22.11864406779662</v>
+        <v>39.237899073120495</v>
       </c>
       <c r="U391" s="1">
-        <v>3.1746031746031775</v>
+        <v>26.666666666666675</v>
       </c>
     </row>
     <row r="392" spans="1:21" x14ac:dyDescent="0.3">
@@ -26092,64 +26095,64 @@
         <v>30</v>
       </c>
       <c r="B395" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C395" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D395" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E395">
-        <v>120</v>
+        <v>85</v>
       </c>
       <c r="F395">
         <v>50</v>
       </c>
       <c r="G395" s="1">
-        <v>27.632950990615218</v>
+        <v>39.140811455847263</v>
       </c>
       <c r="H395" s="1">
-        <v>11.27673608566861</v>
+        <v>13.239460115109472</v>
       </c>
       <c r="I395" s="1">
-        <v>24.940678018522423</v>
+        <v>2.3416369957330652</v>
       </c>
       <c r="J395" s="1">
-        <v>-2.8056785746975885</v>
+        <v>29.320510117936401</v>
       </c>
       <c r="K395" s="1">
-        <v>8.2644628099173563</v>
+        <v>-10.891089108910888</v>
       </c>
       <c r="L395" s="1">
-        <v>21.136991776519732</v>
+        <v>9.6895856360953729</v>
       </c>
       <c r="M395" s="1">
-        <v>5.5493039822680599</v>
+        <v>7.2283297851002297</v>
       </c>
       <c r="N395" s="1">
-        <v>2.5814246016168956</v>
+        <v>8.7975729943756615</v>
       </c>
       <c r="O395" s="1">
-        <v>-12.03241206541051</v>
+        <v>7.7287753134868824</v>
       </c>
       <c r="P395" s="1">
-        <v>-2.6424628792480664</v>
+        <v>1.3899248538075564</v>
       </c>
       <c r="Q395" s="1">
-        <v>-17.343785727686349</v>
+        <v>24.758392155487968</v>
       </c>
       <c r="R395" s="1">
-        <v>1.890608375228958</v>
+        <v>3.0899139937893971</v>
       </c>
       <c r="S395" s="1">
-        <v>21.509121852964203</v>
+        <v>36.359150459036002</v>
       </c>
       <c r="T395" s="1">
-        <v>12.711864406779661</v>
+        <v>17.211538461538471</v>
       </c>
       <c r="U395" s="1">
-        <v>0</v>
+        <v>12.432432432432423</v>
       </c>
     </row>
     <row r="396" spans="1:21" x14ac:dyDescent="0.3">
@@ -26222,64 +26225,64 @@
         <v>30</v>
       </c>
       <c r="B397" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C397" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D397" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E397">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="F397">
-        <v>2.5</v>
+        <v>50</v>
       </c>
       <c r="G397" s="1">
-        <v>16.666666666666668</v>
+        <v>64.75</v>
       </c>
       <c r="H397" s="1">
-        <v>15.946430690037413</v>
+        <v>-31.172531672228612</v>
       </c>
       <c r="I397" s="1">
-        <v>-100.21127578293681</v>
+        <v>-48.760362039503576</v>
       </c>
       <c r="J397" s="1">
-        <v>13.228857943908903</v>
+        <v>-25.878328048769067</v>
       </c>
       <c r="K397" s="1">
-        <v>-13.592233009708723</v>
+        <v>-3.7313432835820897</v>
       </c>
       <c r="L397" s="1">
-        <v>51.100675561797175</v>
+        <v>-30.446323255704296</v>
       </c>
       <c r="M397" s="1">
-        <v>12.838991063745867</v>
+        <v>2.9755468518967647</v>
       </c>
       <c r="N397" s="1">
-        <v>-10.391204507485345</v>
+        <v>-1.0301243516850336</v>
       </c>
       <c r="O397" s="1">
-        <v>-0.18370369950166177</v>
+        <v>-2.7392348718780144</v>
       </c>
       <c r="P397" s="1">
-        <v>-15.135983880256132</v>
+        <v>10.58502628483202</v>
       </c>
       <c r="Q397" s="1">
-        <v>9.8487164969732977</v>
+        <v>-20.81976356248493</v>
       </c>
       <c r="R397" s="1">
-        <v>3.9120154195448538</v>
+        <v>6.3111520246506423</v>
       </c>
       <c r="S397" s="1">
-        <v>13.167816840911437</v>
+        <v>48.691514637815416</v>
       </c>
       <c r="T397" s="1">
-        <v>11.304347826086962</v>
+        <v>-74.107142857142847</v>
       </c>
       <c r="U397" s="1">
-        <v>8.3333333333333321</v>
+        <v>-4.9999999999999973</v>
       </c>
     </row>
     <row r="398" spans="1:21" x14ac:dyDescent="0.3">
@@ -26482,64 +26485,64 @@
         <v>30</v>
       </c>
       <c r="B401" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C401" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D401" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E401">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="F401">
         <v>50</v>
       </c>
       <c r="G401" s="1">
-        <v>43.583333333333336</v>
+        <v>77.592592592592595</v>
       </c>
       <c r="H401" s="1">
-        <v>-15.407263525619065</v>
+        <v>-4.5154096007960698</v>
       </c>
       <c r="I401" s="1">
-        <v>-92.919338327989976</v>
+        <v>32.364468939966528</v>
       </c>
       <c r="J401" s="1">
-        <v>17.171742244010339</v>
+        <v>2.2847280945335569</v>
       </c>
       <c r="K401" s="1">
-        <v>-47.572815533980567</v>
+        <v>-12.213740458015266</v>
       </c>
       <c r="L401" s="1">
-        <v>11.023985463046413</v>
+        <v>9.6192835807068864</v>
       </c>
       <c r="M401" s="1">
-        <v>9.7139899040366888</v>
+        <v>-8.4639890254564119</v>
       </c>
       <c r="N401" s="1">
-        <v>-30.660794822196628</v>
+        <v>-12.848731857680818</v>
       </c>
       <c r="O401" s="1">
-        <v>-25.247757255816882</v>
+        <v>-5.0812585325580271</v>
       </c>
       <c r="P401" s="1">
-        <v>-31.06862871891644</v>
+        <v>6.7962499411558799</v>
       </c>
       <c r="Q401" s="1">
-        <v>4.6818227830371049</v>
+        <v>11.708051053734422</v>
       </c>
       <c r="R401" s="1">
-        <v>10.878465555158414</v>
+        <v>10.606877537239267</v>
       </c>
       <c r="S401" s="1">
-        <v>6.7646660559060487</v>
+        <v>54.226827551063785</v>
       </c>
       <c r="T401" s="1">
-        <v>3.4782608695652204</v>
+        <v>4.3859649122807012</v>
       </c>
       <c r="U401" s="1">
-        <v>-14.393939393939396</v>
+        <v>3.8167938931297711</v>
       </c>
     </row>
     <row r="402" spans="1:21" x14ac:dyDescent="0.3">
@@ -26612,7 +26615,7 @@
         <v>30</v>
       </c>
       <c r="B403" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="C403" t="s">
         <v>29</v>
@@ -26621,55 +26624,55 @@
         <v>35</v>
       </c>
       <c r="E403">
-        <v>127</v>
+        <v>99</v>
       </c>
       <c r="F403">
-        <v>2.5</v>
+        <v>50</v>
       </c>
       <c r="G403" s="1">
-        <v>7.9019073569482297</v>
+        <v>61.904761904761905</v>
       </c>
       <c r="H403" s="1">
-        <v>14.156176776825536</v>
+        <v>-19.550606257123928</v>
       </c>
       <c r="I403" s="1">
-        <v>8.6400782189226177</v>
+        <v>-1.386100088067223</v>
       </c>
       <c r="J403" s="1">
-        <v>11.616904339957685</v>
+        <v>1.5430455347521295</v>
       </c>
       <c r="K403" s="1">
-        <v>-0.94339622641509102</v>
+        <v>-11.586051743532051</v>
       </c>
       <c r="L403" s="1">
-        <v>29.379372774062713</v>
+        <v>6.9246849928859451</v>
       </c>
       <c r="M403" s="1">
-        <v>12.067357017596606</v>
+        <v>4.6893810050200116E-2</v>
       </c>
       <c r="N403" s="1">
-        <v>9.5003198983918775</v>
+        <v>-4.350039664907162E-2</v>
       </c>
       <c r="O403" s="1">
-        <v>7.3684465417796527</v>
+        <v>-6.4344882714734348</v>
       </c>
       <c r="P403" s="1">
-        <v>4.0109213644374364</v>
+        <v>-9.818939222084154</v>
       </c>
       <c r="Q403" s="1">
-        <v>19.882646586574513</v>
+        <v>7.3396519103064026</v>
       </c>
       <c r="R403" s="1">
-        <v>17.838971865909532</v>
+        <v>0.40168194899612775</v>
       </c>
       <c r="S403" s="1">
-        <v>-21.160054060380073</v>
+        <v>37.676866903079031</v>
       </c>
       <c r="T403" s="1">
-        <v>15.412844036697244</v>
+        <v>21.057692307692303</v>
       </c>
       <c r="U403" s="1">
-        <v>6.4220183486238636</v>
+        <v>6.9607843137254823</v>
       </c>
     </row>
     <row r="404" spans="1:21" x14ac:dyDescent="0.3">
@@ -26872,7 +26875,7 @@
         <v>30</v>
       </c>
       <c r="B407" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="C407" t="s">
         <v>29</v>
@@ -26881,55 +26884,55 @@
         <v>35</v>
       </c>
       <c r="E407">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="F407">
         <v>50</v>
       </c>
       <c r="G407" s="1">
-        <v>42.779291553133511</v>
+        <v>48.387096774193544</v>
       </c>
       <c r="H407" s="1">
-        <v>7.5669022207273677</v>
+        <v>16.077995002928894</v>
       </c>
       <c r="I407" s="1">
-        <v>2.5392436628547514</v>
+        <v>15.297664126849131</v>
       </c>
       <c r="J407" s="1">
-        <v>5.5421378238934302</v>
+        <v>9.2944321170583901</v>
       </c>
       <c r="K407" s="1">
         <v>3.773584905660381</v>
       </c>
       <c r="L407" s="1">
-        <v>12.129090137098711</v>
+        <v>8.4191254799941291</v>
       </c>
       <c r="M407" s="1">
-        <v>2.7632601202301856</v>
+        <v>5.4122442068287482</v>
       </c>
       <c r="N407" s="1">
-        <v>-0.83435350360101668</v>
+        <v>17.096461103074201</v>
       </c>
       <c r="O407" s="1">
-        <v>-2.6601536103004326</v>
+        <v>14.611798243799317</v>
       </c>
       <c r="P407" s="1">
-        <v>2.2381055917980621</v>
+        <v>24.232850340135126</v>
       </c>
       <c r="Q407" s="1">
-        <v>2.4499107489143448</v>
+        <v>10.491545018553513</v>
       </c>
       <c r="R407" s="1">
-        <v>6.5274511719421309</v>
+        <v>7.1462695534399572</v>
       </c>
       <c r="S407" s="1">
-        <v>24.397029222625132</v>
+        <v>40.38461538461538</v>
       </c>
       <c r="T407" s="1">
-        <v>15.137614678899086</v>
+        <v>7.3394495412844103</v>
       </c>
       <c r="U407" s="1">
-        <v>17.981651376146797</v>
+        <v>8.4967320261437944</v>
       </c>
     </row>
     <row r="408" spans="1:21" x14ac:dyDescent="0.3">
@@ -27002,64 +27005,64 @@
         <v>30</v>
       </c>
       <c r="B409" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="C409" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D409" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E409">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="F409">
-        <v>2.5</v>
+        <v>50</v>
       </c>
       <c r="G409" s="1">
-        <v>21.874999999999996</v>
+        <v>27.632950990615218</v>
       </c>
       <c r="H409" s="1">
-        <v>16.325073795067652</v>
+        <v>11.27673608566861</v>
       </c>
       <c r="I409" s="1">
-        <v>10.985978119274966</v>
+        <v>24.940678018522423</v>
       </c>
       <c r="J409" s="1">
-        <v>13.521101658507428</v>
+        <v>-2.8056785746975885</v>
       </c>
       <c r="K409" s="1">
-        <v>-2.4340770791075075</v>
+        <v>8.2644628099173563</v>
       </c>
       <c r="L409" s="1">
-        <v>26.314783542392469</v>
+        <v>21.136991776519732</v>
       </c>
       <c r="M409" s="1">
-        <v>6.378174984405816</v>
+        <v>5.5493039822680599</v>
       </c>
       <c r="N409" s="1">
-        <v>17.028724470418581</v>
+        <v>2.5814246016168956</v>
       </c>
       <c r="O409" s="1">
-        <v>3.4056062706377865</v>
+        <v>-12.03241206541051</v>
       </c>
       <c r="P409" s="1">
-        <v>9.8521267526814071</v>
+        <v>-2.6424628792480664</v>
       </c>
       <c r="Q409" s="1">
-        <v>14.1271221847962</v>
+        <v>-17.343785727686349</v>
       </c>
       <c r="R409" s="1">
-        <v>9.5599010082904972</v>
+        <v>1.890608375228958</v>
       </c>
       <c r="S409" s="1">
-        <v>54.981013113053933</v>
+        <v>21.509121852964203</v>
       </c>
       <c r="T409" s="1">
-        <v>3.8293216630197091</v>
+        <v>12.711864406779661</v>
       </c>
       <c r="U409" s="1">
-        <v>9.649122807017541</v>
+        <v>0</v>
       </c>
     </row>
     <row r="410" spans="1:21" x14ac:dyDescent="0.3">
@@ -27262,64 +27265,64 @@
         <v>30</v>
       </c>
       <c r="B413" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="C413" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D413" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E413">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="F413">
         <v>50</v>
       </c>
       <c r="G413" s="1">
-        <v>58.645833333333321</v>
+        <v>43.583333333333336</v>
       </c>
       <c r="H413" s="1">
-        <v>-0.65492495594265843</v>
+        <v>-15.407263525619065</v>
       </c>
       <c r="I413" s="1">
-        <v>-4.0248109538509915</v>
+        <v>-92.919338327989976</v>
       </c>
       <c r="J413" s="1">
-        <v>5.675450582594781</v>
+        <v>17.171742244010339</v>
       </c>
       <c r="K413" s="1">
-        <v>-15.618661257606501</v>
+        <v>-47.572815533980567</v>
       </c>
       <c r="L413" s="1">
-        <v>9.406118706374297</v>
+        <v>11.023985463046413</v>
       </c>
       <c r="M413" s="1">
-        <v>-2.98994662939345</v>
+        <v>9.7139899040366888</v>
       </c>
       <c r="N413" s="1">
-        <v>16.11984359962096</v>
+        <v>-30.660794822196628</v>
       </c>
       <c r="O413" s="1">
-        <v>1.4471724194875606</v>
+        <v>-25.247757255816882</v>
       </c>
       <c r="P413" s="1">
-        <v>7.2957958543330186</v>
+        <v>-31.06862871891644</v>
       </c>
       <c r="Q413" s="1">
-        <v>11.570567230373948</v>
+        <v>4.6818227830371049</v>
       </c>
       <c r="R413" s="1">
-        <v>0.80058203080701418</v>
+        <v>10.878465555158414</v>
       </c>
       <c r="S413" s="1">
-        <v>39.742482057993456</v>
+        <v>6.7646660559060487</v>
       </c>
       <c r="T413" s="1">
-        <v>-5.2516411378555645</v>
+        <v>3.4782608695652204</v>
       </c>
       <c r="U413" s="1">
-        <v>7.0175438596491286</v>
+        <v>-14.393939393939396</v>
       </c>
     </row>
     <row r="414" spans="1:21" x14ac:dyDescent="0.3">
@@ -27395,61 +27398,61 @@
         <v>4</v>
       </c>
       <c r="C415" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D415" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E415">
-        <v>148</v>
+        <v>127</v>
       </c>
       <c r="F415">
-        <v>2.5</v>
+        <v>50</v>
       </c>
       <c r="G415" s="1">
-        <v>38.721804511278194</v>
+        <v>42.779291553133511</v>
       </c>
       <c r="H415" s="1">
-        <v>1.6099461769504189</v>
+        <v>7.5669022207273677</v>
       </c>
       <c r="I415" s="1">
-        <v>-32.030308835050995</v>
+        <v>2.5392436628547514</v>
       </c>
       <c r="J415" s="1">
-        <v>-18.878288525348228</v>
+        <v>5.5421378238934302</v>
       </c>
       <c r="K415" s="1">
-        <v>3.4722222222222223</v>
+        <v>3.773584905660381</v>
       </c>
       <c r="L415" s="1">
-        <v>-7.50466745822765</v>
+        <v>12.129090137098711</v>
       </c>
       <c r="M415" s="1">
-        <v>14.179371347332351</v>
+        <v>2.7632601202301856</v>
       </c>
       <c r="N415" s="1">
-        <v>-7.2122114011544367</v>
+        <v>-0.83435350360101668</v>
       </c>
       <c r="O415" s="1">
-        <v>12.328726143692432</v>
+        <v>-2.6601536103004326</v>
       </c>
       <c r="P415" s="1">
-        <v>-9.2549770111207721</v>
+        <v>2.2381055917980621</v>
       </c>
       <c r="Q415" s="1">
-        <v>-31.877041988105347</v>
+        <v>2.4499107489143448</v>
       </c>
       <c r="R415" s="1">
-        <v>11.802665924220515</v>
+        <v>6.5274511719421309</v>
       </c>
       <c r="S415" s="1">
-        <v>45.455733669659317</v>
+        <v>24.397029222625132</v>
       </c>
       <c r="T415" s="1">
-        <v>2.2727272727272649</v>
+        <v>15.137614678899086</v>
       </c>
       <c r="U415" s="1">
-        <v>12.643678160919539</v>
+        <v>17.981651376146797</v>
       </c>
     </row>
     <row r="416" spans="1:21" x14ac:dyDescent="0.3">
@@ -27655,61 +27658,61 @@
         <v>4</v>
       </c>
       <c r="C419" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D419" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E419">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="F419">
         <v>50</v>
       </c>
       <c r="G419" s="1">
-        <v>37.368421052631582</v>
+        <v>58.645833333333321</v>
       </c>
       <c r="H419" s="1">
-        <v>-2.331456958364595</v>
+        <v>-0.65492495594265843</v>
       </c>
       <c r="I419" s="1">
-        <v>-15.507710966009091</v>
+        <v>-4.0248109538509915</v>
       </c>
       <c r="J419" s="1">
-        <v>-4.2314510179064087</v>
+        <v>5.675450582594781</v>
       </c>
       <c r="K419" s="1">
-        <v>9.0277777777777821</v>
+        <v>-15.618661257606501</v>
       </c>
       <c r="L419" s="1">
-        <v>-0.92977855068330661</v>
+        <v>9.406118706374297</v>
       </c>
       <c r="M419" s="1">
-        <v>12.512612590413335</v>
+        <v>-2.98994662939345</v>
       </c>
       <c r="N419" s="1">
-        <v>-18.396890179187768</v>
+        <v>16.11984359962096</v>
       </c>
       <c r="O419" s="1">
-        <v>13.214431168085166</v>
+        <v>1.4471724194875606</v>
       </c>
       <c r="P419" s="1">
-        <v>-12.342773035692213</v>
+        <v>7.2957958543330186</v>
       </c>
       <c r="Q419" s="1">
-        <v>-10.834603253429103</v>
+        <v>11.570567230373948</v>
       </c>
       <c r="R419" s="1">
-        <v>0.71048786320013946</v>
+        <v>0.80058203080701418</v>
       </c>
       <c r="S419" s="1">
-        <v>58.470984118299576</v>
+        <v>39.742482057993456</v>
       </c>
       <c r="T419" s="1">
-        <v>10.606060606060597</v>
+        <v>-5.2516411378555645</v>
       </c>
       <c r="U419" s="1">
-        <v>9.7701149425287337</v>
+        <v>7.0175438596491286</v>
       </c>
     </row>
     <row r="420" spans="1:21" x14ac:dyDescent="0.3">
@@ -27791,55 +27794,55 @@
         <v>33</v>
       </c>
       <c r="E421">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="F421">
-        <v>2.5</v>
-      </c>
-      <c r="G421" s="1" t="s">
-        <v>20</v>
+        <v>50</v>
+      </c>
+      <c r="G421" s="1">
+        <v>37.368421052631582</v>
       </c>
       <c r="H421" s="1">
-        <v>6.3725677728714798</v>
+        <v>-2.331456958364595</v>
       </c>
       <c r="I421" s="1">
-        <v>-33.22007031576856</v>
+        <v>-15.507710966009091</v>
       </c>
       <c r="J421" s="1">
-        <v>1.5539269591014728</v>
+        <v>-4.2314510179064087</v>
       </c>
       <c r="K421" s="1">
-        <v>-3.2786885245901671</v>
+        <v>9.0277777777777821</v>
       </c>
       <c r="L421" s="1">
-        <v>10.432399260333597</v>
+        <v>-0.92977855068330661</v>
       </c>
       <c r="M421" s="1">
-        <v>5.6320802083774533</v>
+        <v>12.512612590413335</v>
       </c>
       <c r="N421" s="1">
-        <v>-8.3228093953704632E-2</v>
+        <v>-18.396890179187768</v>
       </c>
       <c r="O421" s="1">
-        <v>-77.841296186673645</v>
+        <v>13.214431168085166</v>
       </c>
       <c r="P421" s="1">
-        <v>0.6849410628318815</v>
+        <v>-12.342773035692213</v>
       </c>
       <c r="Q421" s="1">
-        <v>-6.7082997072445112</v>
+        <v>-10.834603253429103</v>
       </c>
       <c r="R421" s="1">
-        <v>3.1790047119904843</v>
+        <v>0.71048786320013946</v>
       </c>
       <c r="S421" s="1">
-        <v>68.277545903157801</v>
+        <v>58.470984118299576</v>
       </c>
       <c r="T421" s="1">
-        <v>11.363636363636365</v>
+        <v>10.606060606060597</v>
       </c>
       <c r="U421" s="1">
-        <v>11.194029850746269</v>
+        <v>9.7701149425287337</v>
       </c>
     </row>
     <row r="422" spans="1:21" x14ac:dyDescent="0.3">
@@ -28103,6 +28106,11 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:U425" xr:uid="{69F37192-1B3F-41AF-BD64-DF8CC03D2933}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A259:U425">
+      <sortCondition ref="F1:F425"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>